<commit_message>
Exe 01 - shape
</commit_message>
<xml_diff>
--- a/me/1.Lap-trinh-python/1.Lap-trinh-python/2.lam-viec-voi-cac-kieu-du-lieu.xlsx
+++ b/me/1.Lap-trinh-python/1.Lap-trinh-python/2.lam-viec-voi-cac-kieu-du-lieu.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vudinhquang/Documents/quang/python/me/1.Lap-trinh-python/1.Lap-trinh-python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F4628AB-9D47-C649-B417-93618CF81908}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F5261F2-9A65-B54A-A829-15597E17FC9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="2200" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{FC6AE9BB-4BEF-564A-A974-1CE698055D30}"/>
+    <workbookView xWindow="3900" yWindow="2200" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{FC6AE9BB-4BEF-564A-A974-1CE698055D30}"/>
   </bookViews>
   <sheets>
     <sheet name="Variable" sheetId="1" r:id="rId1"/>
     <sheet name="Number" sheetId="2" r:id="rId2"/>
+    <sheet name="Exe 01 - shape" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="48">
   <si>
     <t>構成</t>
   </si>
@@ -138,13 +139,95 @@
   </si>
   <si>
     <t>&lt;class 'str'&gt;</t>
+  </si>
+  <si>
+    <t>exe</t>
+  </si>
+  <si>
+    <t>exe_01_shape.py</t>
+  </si>
+  <si>
+    <t>python/exe/exe_01_shape.py</t>
+  </si>
+  <si>
+    <t># Input : Cho chiều dài và chiều rộng của hình chữ nhật</t>
+  </si>
+  <si>
+    <t># Output: Chu vi hình chữ nhật</t>
+  </si>
+  <si>
+    <t>x = 10</t>
+  </si>
+  <si>
+    <t>y = 5</t>
+  </si>
+  <si>
+    <t>result = (x+y) * 2</t>
+  </si>
+  <si>
+    <t>print(x, y, sep=" ", end="\n")</t>
+  </si>
+  <si>
+    <t>print(result)</t>
+  </si>
+  <si>
+    <t>python3 exe_01_shape.py</t>
+  </si>
+  <si>
+    <t>10 5</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">end: string appended after the last value, default a </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>newline</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">step: string inserted between values, default a </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>space</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -158,6 +241,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri (Body)"/>
     </font>
   </fonts>
   <fills count="3">
@@ -266,7 +354,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -279,12 +367,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -390,6 +482,108 @@
         <a:xfrm>
           <a:off x="965200" y="6807200"/>
           <a:ext cx="10689198" cy="1625600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Straight Arrow Connector 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1C4F5333-6087-9469-5A30-C4C661A601C2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="1676400" y="4381500"/>
+          <a:ext cx="4152900" cy="381000"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>111660</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{28D6AC9B-79BC-43AC-3316-D76543030F14}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="939800" y="6184900"/>
+          <a:ext cx="10728860" cy="1270000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -797,7 +991,7 @@
       <c r="E16" t="s">
         <v>13</v>
       </c>
-      <c r="F16" s="14">
+      <c r="F16" s="13">
         <v>1</v>
       </c>
     </row>
@@ -809,7 +1003,7 @@
       <c r="E17" t="s">
         <v>13</v>
       </c>
-      <c r="F17" s="13" t="s">
+      <c r="F17" s="12" t="s">
         <v>31</v>
       </c>
     </row>
@@ -933,8 +1127,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B0CC97E-5A37-2E41-A870-EAFA42883709}">
   <dimension ref="A4:O42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1010,35 +1204,27 @@
       <c r="B16" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
       <c r="E16" s="5"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B17" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
       <c r="E17" s="5"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B18" s="4"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
       <c r="E18" s="5"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B19" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
       <c r="E19" s="5"/>
       <c r="F19" t="s">
         <v>13</v>
       </c>
-      <c r="G19" s="14">
+      <c r="G19" s="13">
         <v>3</v>
       </c>
     </row>
@@ -1046,68 +1232,54 @@
       <c r="B20" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
       <c r="E20" s="5"/>
       <c r="F20" t="s">
         <v>13</v>
       </c>
-      <c r="G20" s="14">
+      <c r="G20" s="13">
         <v>160</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B21" s="4"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
       <c r="E21" s="5"/>
-      <c r="G21" s="14"/>
+      <c r="G21" s="13"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B22" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C22" s="12"/>
-      <c r="D22" s="12"/>
       <c r="E22" s="5"/>
-      <c r="G22" s="14"/>
+      <c r="G22" s="13"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B23" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C23" s="12"/>
-      <c r="D23" s="12"/>
       <c r="E23" s="5"/>
-      <c r="G23" s="14"/>
+      <c r="G23" s="13"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B24" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C24" s="12"/>
-      <c r="D24" s="12"/>
       <c r="E24" s="5"/>
-      <c r="G24" s="14"/>
+      <c r="G24" s="13"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B25" s="4"/>
-      <c r="C25" s="12"/>
-      <c r="D25" s="12"/>
       <c r="E25" s="5"/>
-      <c r="G25" s="14"/>
+      <c r="G25" s="13"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B26" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C26" s="12"/>
-      <c r="D26" s="12"/>
       <c r="E26" s="5"/>
       <c r="F26" t="s">
         <v>13</v>
       </c>
-      <c r="G26" s="14">
+      <c r="G26" s="13">
         <v>2</v>
       </c>
     </row>
@@ -1115,13 +1287,11 @@
       <c r="B27" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C27" s="12"/>
-      <c r="D27" s="12"/>
       <c r="E27" s="5"/>
       <c r="F27" t="s">
         <v>13</v>
       </c>
-      <c r="G27" s="14">
+      <c r="G27" s="13">
         <v>2.2999999999999998</v>
       </c>
     </row>
@@ -1129,8 +1299,6 @@
       <c r="B28" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C28" s="12"/>
-      <c r="D28" s="12"/>
       <c r="E28" s="5"/>
       <c r="F28" t="s">
         <v>13</v>
@@ -1166,157 +1334,41 @@
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A33" s="4"/>
-      <c r="B33" s="12" t="s">
+      <c r="B33" t="s">
         <v>29</v>
       </c>
-      <c r="C33" s="12"/>
-      <c r="D33" s="12"/>
-      <c r="E33" s="12"/>
-      <c r="F33" s="12"/>
-      <c r="G33" s="12"/>
-      <c r="H33" s="12"/>
-      <c r="I33" s="12"/>
-      <c r="J33" s="12"/>
-      <c r="K33" s="12"/>
-      <c r="L33" s="12"/>
-      <c r="M33" s="12"/>
-      <c r="N33" s="12"/>
       <c r="O33" s="5"/>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A34" s="4"/>
-      <c r="B34" s="12"/>
-      <c r="C34" s="12"/>
-      <c r="D34" s="12"/>
-      <c r="E34" s="12"/>
-      <c r="F34" s="12"/>
-      <c r="G34" s="12"/>
-      <c r="H34" s="12"/>
-      <c r="I34" s="12"/>
-      <c r="J34" s="12"/>
-      <c r="K34" s="12"/>
-      <c r="L34" s="12"/>
-      <c r="M34" s="12"/>
-      <c r="N34" s="12"/>
       <c r="O34" s="5"/>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A35" s="4"/>
-      <c r="B35" s="12"/>
-      <c r="C35" s="12"/>
-      <c r="D35" s="12"/>
-      <c r="E35" s="12"/>
-      <c r="F35" s="12"/>
-      <c r="G35" s="12"/>
-      <c r="H35" s="12"/>
-      <c r="I35" s="12"/>
-      <c r="J35" s="12"/>
-      <c r="K35" s="12"/>
-      <c r="L35" s="12"/>
-      <c r="M35" s="12"/>
-      <c r="N35" s="12"/>
       <c r="O35" s="5"/>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A36" s="4"/>
-      <c r="B36" s="12"/>
-      <c r="C36" s="12"/>
-      <c r="D36" s="12"/>
-      <c r="E36" s="12"/>
-      <c r="F36" s="12"/>
-      <c r="G36" s="12"/>
-      <c r="H36" s="12"/>
-      <c r="I36" s="12"/>
-      <c r="J36" s="12"/>
-      <c r="K36" s="12"/>
-      <c r="L36" s="12"/>
-      <c r="M36" s="12"/>
-      <c r="N36" s="12"/>
       <c r="O36" s="5"/>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A37" s="4"/>
-      <c r="B37" s="12"/>
-      <c r="C37" s="12"/>
-      <c r="D37" s="12"/>
-      <c r="E37" s="12"/>
-      <c r="F37" s="12"/>
-      <c r="G37" s="12"/>
-      <c r="H37" s="12"/>
-      <c r="I37" s="12"/>
-      <c r="J37" s="12"/>
-      <c r="K37" s="12"/>
-      <c r="L37" s="12"/>
-      <c r="M37" s="12"/>
-      <c r="N37" s="12"/>
       <c r="O37" s="5"/>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A38" s="4"/>
-      <c r="B38" s="12"/>
-      <c r="C38" s="12"/>
-      <c r="D38" s="12"/>
-      <c r="E38" s="12"/>
-      <c r="F38" s="12"/>
-      <c r="G38" s="12"/>
-      <c r="H38" s="12"/>
-      <c r="I38" s="12"/>
-      <c r="J38" s="12"/>
-      <c r="K38" s="12"/>
-      <c r="L38" s="12"/>
-      <c r="M38" s="12"/>
-      <c r="N38" s="12"/>
       <c r="O38" s="5"/>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A39" s="4"/>
-      <c r="B39" s="12"/>
-      <c r="C39" s="12"/>
-      <c r="D39" s="12"/>
-      <c r="E39" s="12"/>
-      <c r="F39" s="12"/>
-      <c r="G39" s="12"/>
-      <c r="H39" s="12"/>
-      <c r="I39" s="12"/>
-      <c r="J39" s="12"/>
-      <c r="K39" s="12"/>
-      <c r="L39" s="12"/>
-      <c r="M39" s="12"/>
-      <c r="N39" s="12"/>
       <c r="O39" s="5"/>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A40" s="4"/>
-      <c r="B40" s="12"/>
-      <c r="C40" s="12"/>
-      <c r="D40" s="12"/>
-      <c r="E40" s="12"/>
-      <c r="F40" s="12"/>
-      <c r="G40" s="12"/>
-      <c r="H40" s="12"/>
-      <c r="I40" s="12"/>
-      <c r="J40" s="12"/>
-      <c r="K40" s="12"/>
-      <c r="L40" s="12"/>
-      <c r="M40" s="12"/>
-      <c r="N40" s="12"/>
       <c r="O40" s="5"/>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A41" s="4"/>
-      <c r="B41" s="12"/>
-      <c r="C41" s="12"/>
-      <c r="D41" s="12"/>
-      <c r="E41" s="12"/>
-      <c r="F41" s="12"/>
-      <c r="G41" s="12"/>
-      <c r="H41" s="12"/>
-      <c r="I41" s="12"/>
-      <c r="J41" s="12"/>
-      <c r="K41" s="12"/>
-      <c r="L41" s="12"/>
-      <c r="M41" s="12"/>
-      <c r="N41" s="12"/>
       <c r="O41" s="5"/>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.2">
@@ -1340,4 +1392,355 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1470482B-3A2C-E741-8F43-420B40AD46DB}">
+  <dimension ref="A4:O37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M24" sqref="M24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="3"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B6" s="4"/>
+      <c r="C6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" s="5"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B7" s="4"/>
+      <c r="D7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7" s="5"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B8" s="4"/>
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" s="5"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B9" s="4"/>
+      <c r="D9" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="F9" s="5"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B10" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="9"/>
+      <c r="F10" s="5"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B11" s="4"/>
+      <c r="C11" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="9"/>
+      <c r="F11" s="5"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B12" s="6"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="8"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B16" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="3"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B17" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="5"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B18" s="4"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="5"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B19" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="5"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B20" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="5"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B21" s="4"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="5"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B22" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22" s="15"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="5"/>
+      <c r="H22" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B23" s="4"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="5"/>
+      <c r="H23" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B24" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C24" s="15"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="5"/>
+      <c r="G24" t="s">
+        <v>13</v>
+      </c>
+      <c r="H24" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B25" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C25" s="15"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="5"/>
+      <c r="G25" t="s">
+        <v>13</v>
+      </c>
+      <c r="H25" s="16">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B26" s="6"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="8"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A29" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="2"/>
+      <c r="L29" s="2"/>
+      <c r="M29" s="2"/>
+      <c r="N29" s="2"/>
+      <c r="O29" s="3"/>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A30" s="4"/>
+      <c r="B30" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="C30" s="15"/>
+      <c r="D30" s="15"/>
+      <c r="E30" s="15"/>
+      <c r="F30" s="15"/>
+      <c r="G30" s="15"/>
+      <c r="H30" s="15"/>
+      <c r="I30" s="15"/>
+      <c r="J30" s="15"/>
+      <c r="K30" s="15"/>
+      <c r="L30" s="15"/>
+      <c r="M30" s="15"/>
+      <c r="N30" s="15"/>
+      <c r="O30" s="5"/>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A31" s="4"/>
+      <c r="B31" s="15"/>
+      <c r="C31" s="15"/>
+      <c r="D31" s="15"/>
+      <c r="E31" s="15"/>
+      <c r="F31" s="15"/>
+      <c r="G31" s="15"/>
+      <c r="H31" s="15"/>
+      <c r="I31" s="15"/>
+      <c r="J31" s="15"/>
+      <c r="K31" s="15"/>
+      <c r="L31" s="15"/>
+      <c r="M31" s="15"/>
+      <c r="N31" s="15"/>
+      <c r="O31" s="5"/>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A32" s="4"/>
+      <c r="B32" s="15"/>
+      <c r="C32" s="15"/>
+      <c r="D32" s="15"/>
+      <c r="E32" s="15"/>
+      <c r="F32" s="15"/>
+      <c r="G32" s="15"/>
+      <c r="H32" s="15"/>
+      <c r="I32" s="15"/>
+      <c r="J32" s="15"/>
+      <c r="K32" s="15"/>
+      <c r="L32" s="15"/>
+      <c r="M32" s="15"/>
+      <c r="N32" s="15"/>
+      <c r="O32" s="5"/>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A33" s="4"/>
+      <c r="B33" s="15"/>
+      <c r="C33" s="15"/>
+      <c r="D33" s="15"/>
+      <c r="E33" s="15"/>
+      <c r="F33" s="15"/>
+      <c r="G33" s="15"/>
+      <c r="H33" s="15"/>
+      <c r="I33" s="15"/>
+      <c r="J33" s="15"/>
+      <c r="K33" s="15"/>
+      <c r="L33" s="15"/>
+      <c r="M33" s="15"/>
+      <c r="N33" s="15"/>
+      <c r="O33" s="5"/>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A34" s="4"/>
+      <c r="B34" s="15"/>
+      <c r="C34" s="15"/>
+      <c r="D34" s="15"/>
+      <c r="E34" s="15"/>
+      <c r="F34" s="15"/>
+      <c r="G34" s="15"/>
+      <c r="H34" s="15"/>
+      <c r="I34" s="15"/>
+      <c r="J34" s="15"/>
+      <c r="K34" s="15"/>
+      <c r="L34" s="15"/>
+      <c r="M34" s="15"/>
+      <c r="N34" s="15"/>
+      <c r="O34" s="5"/>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A35" s="4"/>
+      <c r="B35" s="15"/>
+      <c r="C35" s="15"/>
+      <c r="D35" s="15"/>
+      <c r="E35" s="15"/>
+      <c r="F35" s="15"/>
+      <c r="G35" s="15"/>
+      <c r="H35" s="15"/>
+      <c r="I35" s="15"/>
+      <c r="J35" s="15"/>
+      <c r="K35" s="15"/>
+      <c r="L35" s="15"/>
+      <c r="M35" s="15"/>
+      <c r="N35" s="15"/>
+      <c r="O35" s="5"/>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A36" s="4"/>
+      <c r="B36" s="15"/>
+      <c r="C36" s="15"/>
+      <c r="D36" s="15"/>
+      <c r="E36" s="15"/>
+      <c r="F36" s="15"/>
+      <c r="G36" s="15"/>
+      <c r="H36" s="15"/>
+      <c r="I36" s="15"/>
+      <c r="J36" s="15"/>
+      <c r="K36" s="15"/>
+      <c r="L36" s="15"/>
+      <c r="M36" s="15"/>
+      <c r="N36" s="15"/>
+      <c r="O36" s="5"/>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A37" s="6"/>
+      <c r="B37" s="7"/>
+      <c r="C37" s="7"/>
+      <c r="D37" s="7"/>
+      <c r="E37" s="7"/>
+      <c r="F37" s="7"/>
+      <c r="G37" s="7"/>
+      <c r="H37" s="7"/>
+      <c r="I37" s="7"/>
+      <c r="J37" s="7"/>
+      <c r="K37" s="7"/>
+      <c r="L37" s="7"/>
+      <c r="M37" s="7"/>
+      <c r="N37" s="7"/>
+      <c r="O37" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Exe 02 - swap
</commit_message>
<xml_diff>
--- a/me/1.Lap-trinh-python/1.Lap-trinh-python/2.lam-viec-voi-cac-kieu-du-lieu.xlsx
+++ b/me/1.Lap-trinh-python/1.Lap-trinh-python/2.lam-viec-voi-cac-kieu-du-lieu.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vudinhquang/Documents/quang/python/me/1.Lap-trinh-python/1.Lap-trinh-python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ED681C5-80D9-6245-936E-76AC77299F4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E8A0710-7B64-C142-AD1D-AF665991E2DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="2200" windowWidth="28040" windowHeight="17440" activeTab="4" xr2:uid="{FC6AE9BB-4BEF-564A-A974-1CE698055D30}"/>
+    <workbookView xWindow="3900" yWindow="2200" windowWidth="28040" windowHeight="17440" activeTab="5" xr2:uid="{FC6AE9BB-4BEF-564A-A974-1CE698055D30}"/>
   </bookViews>
   <sheets>
     <sheet name="Variable" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Exe 01 - shape" sheetId="3" r:id="rId3"/>
     <sheet name="String 01" sheetId="4" r:id="rId4"/>
     <sheet name="String 02" sheetId="5" r:id="rId5"/>
+    <sheet name="Exe 02 - swap" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="110">
   <si>
     <t>構成</t>
   </si>
@@ -370,6 +371,45 @@
   </si>
   <si>
     <t>result7 = myStr[::3] # Không truyền from và to, có bước nhảy là 3 -&gt; hlph</t>
+  </si>
+  <si>
+    <t>exe_02_swap.py</t>
+  </si>
+  <si>
+    <t>python/exe/exe_02_swap.py</t>
+  </si>
+  <si>
+    <t># Input : Cho 2 chuỗi x = "abc", y = "xyz"</t>
+  </si>
+  <si>
+    <t># Output: Tạo ra chuỗi mới xyc abz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                        </t>
+  </si>
+  <si>
+    <t>x = "abc"</t>
+  </si>
+  <si>
+    <t>y = "xyz"</t>
+  </si>
+  <si>
+    <t>xNew = y[:len(y)-1] + x[-1]</t>
+  </si>
+  <si>
+    <t>yNew = x[:len(x)-1] + y[-1]</t>
+  </si>
+  <si>
+    <t>result = xNew + " " + yNew</t>
+  </si>
+  <si>
+    <t>python3 exe_02_swap.py</t>
+  </si>
+  <si>
+    <t>xyc</t>
+  </si>
+  <si>
+    <t>abz</t>
   </si>
 </sst>
 </file>
@@ -503,7 +543,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -529,6 +569,8 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -784,6 +826,104 @@
         <a:xfrm>
           <a:off x="939800" y="11252200"/>
           <a:ext cx="10312400" cy="1856232"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>101600</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>606054</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FA3F9DE4-326F-2623-D4B0-636DE7D551C8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="927100" y="14274800"/>
+          <a:ext cx="11235954" cy="3073400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>101600</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>191894</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{69378BE6-36B8-D154-2643-78EFE548ADA2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="927100" y="6794500"/>
+          <a:ext cx="9996294" cy="1003300"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2279,10 +2419,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BE2AFA6-DD22-5A4F-A8A5-AB93BD207990}">
-  <dimension ref="A3:J66"/>
+  <dimension ref="A3:O86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="N41" sqref="N41"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="H58" sqref="H58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2695,7 +2835,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="65" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B65" s="16" t="s">
         <v>89</v>
       </c>
@@ -2703,7 +2843,7 @@
       <c r="I65" s="13"/>
       <c r="J65" s="13"/>
     </row>
-    <row r="66" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B66" s="6"/>
       <c r="C66" s="7"/>
       <c r="D66" s="7"/>
@@ -2712,7 +2852,662 @@
       <c r="G66" s="7"/>
       <c r="H66" s="8"/>
     </row>
+    <row r="69" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A69" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B69" s="2"/>
+      <c r="C69" s="2"/>
+      <c r="D69" s="2"/>
+      <c r="E69" s="2"/>
+      <c r="F69" s="2"/>
+      <c r="G69" s="2"/>
+      <c r="H69" s="2"/>
+      <c r="I69" s="2"/>
+      <c r="J69" s="2"/>
+      <c r="K69" s="2"/>
+      <c r="L69" s="2"/>
+      <c r="M69" s="2"/>
+      <c r="N69" s="2"/>
+      <c r="O69" s="3"/>
+    </row>
+    <row r="70" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A70" s="4"/>
+      <c r="B70" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="C70" s="18"/>
+      <c r="D70" s="18"/>
+      <c r="E70" s="18"/>
+      <c r="F70" s="18"/>
+      <c r="G70" s="18"/>
+      <c r="H70" s="18"/>
+      <c r="I70" s="18"/>
+      <c r="J70" s="18"/>
+      <c r="K70" s="18"/>
+      <c r="L70" s="18"/>
+      <c r="M70" s="18"/>
+      <c r="N70" s="18"/>
+      <c r="O70" s="5"/>
+    </row>
+    <row r="71" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A71" s="4"/>
+      <c r="B71" s="18"/>
+      <c r="C71" s="18"/>
+      <c r="D71" s="18"/>
+      <c r="E71" s="18"/>
+      <c r="F71" s="18"/>
+      <c r="G71" s="18"/>
+      <c r="H71" s="18"/>
+      <c r="I71" s="18"/>
+      <c r="J71" s="18"/>
+      <c r="K71" s="18"/>
+      <c r="L71" s="18"/>
+      <c r="M71" s="18"/>
+      <c r="N71" s="18"/>
+      <c r="O71" s="5"/>
+    </row>
+    <row r="72" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A72" s="4"/>
+      <c r="B72" s="18"/>
+      <c r="C72" s="18"/>
+      <c r="D72" s="18"/>
+      <c r="E72" s="18"/>
+      <c r="F72" s="18"/>
+      <c r="G72" s="18"/>
+      <c r="H72" s="18"/>
+      <c r="I72" s="18"/>
+      <c r="J72" s="18"/>
+      <c r="K72" s="18"/>
+      <c r="L72" s="18"/>
+      <c r="M72" s="18"/>
+      <c r="N72" s="18"/>
+      <c r="O72" s="5"/>
+    </row>
+    <row r="73" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A73" s="4"/>
+      <c r="B73" s="18"/>
+      <c r="C73" s="18"/>
+      <c r="D73" s="18"/>
+      <c r="E73" s="18"/>
+      <c r="F73" s="18"/>
+      <c r="G73" s="18"/>
+      <c r="H73" s="18"/>
+      <c r="I73" s="18"/>
+      <c r="J73" s="18"/>
+      <c r="K73" s="18"/>
+      <c r="L73" s="18"/>
+      <c r="M73" s="18"/>
+      <c r="N73" s="18"/>
+      <c r="O73" s="5"/>
+    </row>
+    <row r="74" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A74" s="4"/>
+      <c r="B74" s="18"/>
+      <c r="C74" s="18"/>
+      <c r="D74" s="18"/>
+      <c r="E74" s="18"/>
+      <c r="F74" s="18"/>
+      <c r="G74" s="18"/>
+      <c r="H74" s="18"/>
+      <c r="I74" s="18"/>
+      <c r="J74" s="18"/>
+      <c r="K74" s="18"/>
+      <c r="L74" s="18"/>
+      <c r="M74" s="18"/>
+      <c r="N74" s="18"/>
+      <c r="O74" s="5"/>
+    </row>
+    <row r="75" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A75" s="4"/>
+      <c r="B75" s="18"/>
+      <c r="C75" s="18"/>
+      <c r="D75" s="18"/>
+      <c r="E75" s="18"/>
+      <c r="F75" s="18"/>
+      <c r="G75" s="18"/>
+      <c r="H75" s="18"/>
+      <c r="I75" s="18"/>
+      <c r="J75" s="18"/>
+      <c r="K75" s="18"/>
+      <c r="L75" s="18"/>
+      <c r="M75" s="18"/>
+      <c r="N75" s="18"/>
+      <c r="O75" s="5"/>
+    </row>
+    <row r="76" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A76" s="4"/>
+      <c r="B76" s="18"/>
+      <c r="C76" s="18"/>
+      <c r="D76" s="18"/>
+      <c r="E76" s="18"/>
+      <c r="F76" s="18"/>
+      <c r="G76" s="18"/>
+      <c r="H76" s="18"/>
+      <c r="I76" s="18"/>
+      <c r="J76" s="18"/>
+      <c r="K76" s="18"/>
+      <c r="L76" s="18"/>
+      <c r="M76" s="18"/>
+      <c r="N76" s="18"/>
+      <c r="O76" s="5"/>
+    </row>
+    <row r="77" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A77" s="4"/>
+      <c r="B77" s="18"/>
+      <c r="C77" s="18"/>
+      <c r="D77" s="18"/>
+      <c r="E77" s="18"/>
+      <c r="F77" s="18"/>
+      <c r="G77" s="18"/>
+      <c r="H77" s="18"/>
+      <c r="I77" s="18"/>
+      <c r="J77" s="18"/>
+      <c r="K77" s="18"/>
+      <c r="L77" s="18"/>
+      <c r="M77" s="18"/>
+      <c r="N77" s="18"/>
+      <c r="O77" s="5"/>
+    </row>
+    <row r="78" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A78" s="4"/>
+      <c r="B78" s="18"/>
+      <c r="C78" s="18"/>
+      <c r="D78" s="18"/>
+      <c r="E78" s="18"/>
+      <c r="F78" s="18"/>
+      <c r="G78" s="18"/>
+      <c r="H78" s="18"/>
+      <c r="I78" s="18"/>
+      <c r="J78" s="18"/>
+      <c r="K78" s="18"/>
+      <c r="L78" s="18"/>
+      <c r="M78" s="18"/>
+      <c r="N78" s="18"/>
+      <c r="O78" s="5"/>
+    </row>
+    <row r="79" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A79" s="4"/>
+      <c r="B79" s="18"/>
+      <c r="C79" s="18"/>
+      <c r="D79" s="18"/>
+      <c r="E79" s="18"/>
+      <c r="F79" s="18"/>
+      <c r="G79" s="18"/>
+      <c r="H79" s="18"/>
+      <c r="I79" s="18"/>
+      <c r="J79" s="18"/>
+      <c r="K79" s="18"/>
+      <c r="L79" s="18"/>
+      <c r="M79" s="18"/>
+      <c r="N79" s="18"/>
+      <c r="O79" s="5"/>
+    </row>
+    <row r="80" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A80" s="4"/>
+      <c r="B80" s="18"/>
+      <c r="C80" s="18"/>
+      <c r="D80" s="18"/>
+      <c r="E80" s="18"/>
+      <c r="F80" s="18"/>
+      <c r="G80" s="18"/>
+      <c r="H80" s="18"/>
+      <c r="I80" s="18"/>
+      <c r="J80" s="18"/>
+      <c r="K80" s="18"/>
+      <c r="L80" s="18"/>
+      <c r="M80" s="18"/>
+      <c r="N80" s="18"/>
+      <c r="O80" s="5"/>
+    </row>
+    <row r="81" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A81" s="4"/>
+      <c r="B81" s="18"/>
+      <c r="C81" s="18"/>
+      <c r="D81" s="18"/>
+      <c r="E81" s="18"/>
+      <c r="F81" s="18"/>
+      <c r="G81" s="18"/>
+      <c r="H81" s="18"/>
+      <c r="I81" s="18"/>
+      <c r="J81" s="18"/>
+      <c r="K81" s="18"/>
+      <c r="L81" s="18"/>
+      <c r="M81" s="18"/>
+      <c r="N81" s="18"/>
+      <c r="O81" s="5"/>
+    </row>
+    <row r="82" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A82" s="4"/>
+      <c r="B82" s="18"/>
+      <c r="C82" s="18"/>
+      <c r="D82" s="18"/>
+      <c r="E82" s="18"/>
+      <c r="F82" s="18"/>
+      <c r="G82" s="18"/>
+      <c r="H82" s="18"/>
+      <c r="I82" s="18"/>
+      <c r="J82" s="18"/>
+      <c r="K82" s="18"/>
+      <c r="L82" s="18"/>
+      <c r="M82" s="18"/>
+      <c r="N82" s="18"/>
+      <c r="O82" s="5"/>
+    </row>
+    <row r="83" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A83" s="4"/>
+      <c r="B83" s="18"/>
+      <c r="C83" s="18"/>
+      <c r="D83" s="18"/>
+      <c r="E83" s="18"/>
+      <c r="F83" s="18"/>
+      <c r="G83" s="18"/>
+      <c r="H83" s="18"/>
+      <c r="I83" s="18"/>
+      <c r="J83" s="18"/>
+      <c r="K83" s="18"/>
+      <c r="L83" s="18"/>
+      <c r="M83" s="18"/>
+      <c r="N83" s="18"/>
+      <c r="O83" s="5"/>
+    </row>
+    <row r="84" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A84" s="4"/>
+      <c r="B84" s="18"/>
+      <c r="C84" s="18"/>
+      <c r="D84" s="18"/>
+      <c r="E84" s="18"/>
+      <c r="F84" s="18"/>
+      <c r="G84" s="18"/>
+      <c r="H84" s="18"/>
+      <c r="I84" s="18"/>
+      <c r="J84" s="18"/>
+      <c r="K84" s="18"/>
+      <c r="L84" s="18"/>
+      <c r="M84" s="18"/>
+      <c r="N84" s="18"/>
+      <c r="O84" s="5"/>
+    </row>
+    <row r="85" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A85" s="4"/>
+      <c r="B85" s="18"/>
+      <c r="C85" s="18"/>
+      <c r="D85" s="18"/>
+      <c r="E85" s="18"/>
+      <c r="F85" s="18"/>
+      <c r="G85" s="18"/>
+      <c r="H85" s="18"/>
+      <c r="I85" s="18"/>
+      <c r="J85" s="18"/>
+      <c r="K85" s="18"/>
+      <c r="L85" s="18"/>
+      <c r="M85" s="18"/>
+      <c r="N85" s="18"/>
+      <c r="O85" s="5"/>
+    </row>
+    <row r="86" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A86" s="6"/>
+      <c r="B86" s="7"/>
+      <c r="C86" s="7"/>
+      <c r="D86" s="7"/>
+      <c r="E86" s="7"/>
+      <c r="F86" s="7"/>
+      <c r="G86" s="7"/>
+      <c r="H86" s="7"/>
+      <c r="I86" s="7"/>
+      <c r="J86" s="7"/>
+      <c r="K86" s="7"/>
+      <c r="L86" s="7"/>
+      <c r="M86" s="7"/>
+      <c r="N86" s="7"/>
+      <c r="O86" s="8"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6143AAC-151D-8845-AE79-4A19DBC41CDB}">
+  <dimension ref="A3:N39"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="H43" sqref="H43"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="3"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B5" s="4"/>
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="5"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B6" s="4"/>
+      <c r="D6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" s="5"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B7" s="4"/>
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" s="5"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B8" s="4"/>
+      <c r="D8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" s="5"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B9" s="4"/>
+      <c r="D9" t="s">
+        <v>48</v>
+      </c>
+      <c r="F9" s="5"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B10" s="4"/>
+      <c r="D10" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="F10" s="5"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B11" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F11" s="5"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B12" s="4"/>
+      <c r="C12" t="s">
+        <v>35</v>
+      </c>
+      <c r="F12" s="5"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B13" s="4"/>
+      <c r="C13" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="F13" s="5"/>
+      <c r="G13" t="s">
+        <v>13</v>
+      </c>
+      <c r="H13" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B14" s="6"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="8"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A17" s="10" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B18" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="3"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B19" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="5"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B20" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="5"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B21" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="5"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B22" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="5"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B23" s="4"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="5"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B24" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="5"/>
+      <c r="F24" t="s">
+        <v>13</v>
+      </c>
+      <c r="G24" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B25" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="5"/>
+      <c r="F25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G25" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B26" s="4"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="5"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B27" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="5"/>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B28" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="5"/>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B29" s="6"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="8"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A32" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
+      <c r="J32" s="2"/>
+      <c r="K32" s="2"/>
+      <c r="L32" s="2"/>
+      <c r="M32" s="2"/>
+      <c r="N32" s="3"/>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A33" s="4"/>
+      <c r="B33" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="18"/>
+      <c r="H33" s="18"/>
+      <c r="I33" s="18"/>
+      <c r="J33" s="18"/>
+      <c r="K33" s="18"/>
+      <c r="L33" s="18"/>
+      <c r="M33" s="18"/>
+      <c r="N33" s="5"/>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A34" s="4"/>
+      <c r="B34" s="18"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="18"/>
+      <c r="H34" s="18"/>
+      <c r="I34" s="18"/>
+      <c r="J34" s="18"/>
+      <c r="K34" s="18"/>
+      <c r="L34" s="18"/>
+      <c r="M34" s="18"/>
+      <c r="N34" s="5"/>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A35" s="4"/>
+      <c r="B35" s="18"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="18"/>
+      <c r="H35" s="18"/>
+      <c r="I35" s="18"/>
+      <c r="J35" s="18"/>
+      <c r="K35" s="18"/>
+      <c r="L35" s="18"/>
+      <c r="M35" s="18"/>
+      <c r="N35" s="5"/>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A36" s="4"/>
+      <c r="B36" s="18"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="18"/>
+      <c r="H36" s="18"/>
+      <c r="I36" s="18"/>
+      <c r="J36" s="18"/>
+      <c r="K36" s="18"/>
+      <c r="L36" s="18"/>
+      <c r="M36" s="18"/>
+      <c r="N36" s="5"/>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A37" s="4"/>
+      <c r="B37" s="18"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="18"/>
+      <c r="G37" s="18"/>
+      <c r="H37" s="18"/>
+      <c r="I37" s="18"/>
+      <c r="J37" s="18"/>
+      <c r="K37" s="18"/>
+      <c r="L37" s="18"/>
+      <c r="M37" s="18"/>
+      <c r="N37" s="5"/>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A38" s="4"/>
+      <c r="B38" s="18"/>
+      <c r="C38" s="18"/>
+      <c r="D38" s="18"/>
+      <c r="E38" s="18"/>
+      <c r="F38" s="18"/>
+      <c r="G38" s="18"/>
+      <c r="H38" s="18"/>
+      <c r="I38" s="18"/>
+      <c r="J38" s="18"/>
+      <c r="K38" s="18"/>
+      <c r="L38" s="18"/>
+      <c r="M38" s="18"/>
+      <c r="N38" s="5"/>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A39" s="6"/>
+      <c r="B39" s="7"/>
+      <c r="C39" s="7"/>
+      <c r="D39" s="7"/>
+      <c r="E39" s="7"/>
+      <c r="F39" s="7"/>
+      <c r="G39" s="7"/>
+      <c r="H39" s="7"/>
+      <c r="I39" s="7"/>
+      <c r="J39" s="7"/>
+      <c r="K39" s="7"/>
+      <c r="L39" s="7"/>
+      <c r="M39" s="7"/>
+      <c r="N39" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Exe 03 - birthday
</commit_message>
<xml_diff>
--- a/me/1.Lap-trinh-python/1.Lap-trinh-python/2.lam-viec-voi-cac-kieu-du-lieu.xlsx
+++ b/me/1.Lap-trinh-python/1.Lap-trinh-python/2.lam-viec-voi-cac-kieu-du-lieu.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vudinhquang/Documents/quang/python/me/1.Lap-trinh-python/1.Lap-trinh-python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE50F135-8FF2-8F45-A43F-BE46C8C12C6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A44A7B3-D1C2-E844-9FEB-E152DC4AFEE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1260" windowWidth="31460" windowHeight="18720" activeTab="8" xr2:uid="{FC6AE9BB-4BEF-564A-A974-1CE698055D30}"/>
+    <workbookView xWindow="1560" yWindow="1260" windowWidth="31460" windowHeight="18720" activeTab="9" xr2:uid="{FC6AE9BB-4BEF-564A-A974-1CE698055D30}"/>
   </bookViews>
   <sheets>
     <sheet name="Variable" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,7 @@
     <sheet name="String 03" sheetId="7" r:id="rId7"/>
     <sheet name="String 04" sheetId="8" r:id="rId8"/>
     <sheet name="String 05" sheetId="9" r:id="rId9"/>
+    <sheet name="Exe 03 - birthday" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="182">
   <si>
     <t>構成</t>
   </si>
@@ -607,6 +608,48 @@
       </rPr>
       <t xml:space="preserve"> ký tự</t>
     </r>
+  </si>
+  <si>
+    <t>exe_03_birthday.py</t>
+  </si>
+  <si>
+    <t>python/exe/exe_03_birthday.py</t>
+  </si>
+  <si>
+    <t># Input : Nhập vào tên và năm sinh</t>
+  </si>
+  <si>
+    <t># Output: Xin chào [name], năm nay bạn [age] tuổi</t>
+  </si>
+  <si>
+    <t># python get current year</t>
+  </si>
+  <si>
+    <t># https://stackoverflow.com/questions/28189442/datetime-current-year-and-month-python/28189525</t>
+  </si>
+  <si>
+    <t># - năm hiện tại</t>
+  </si>
+  <si>
+    <t># - lấy giá trị mà người dùng họ nhập vào</t>
+  </si>
+  <si>
+    <t>from datetime import datetime</t>
+  </si>
+  <si>
+    <t>currentYear = datetime.now().year</t>
+  </si>
+  <si>
+    <t>name        = input("Nhập vào tên của bạn: ")</t>
+  </si>
+  <si>
+    <t>birthday    = int(input("Nhập vào năm sinh của bạn: "))</t>
+  </si>
+  <si>
+    <t>result      = "Xin chào {name}, năm nay bạn {age} tuổi".format(name=name, age = currentYear - birthday)</t>
+  </si>
+  <si>
+    <t>python3 exe_03_birthday.py</t>
   </si>
 </sst>
 </file>
@@ -774,9 +817,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -838,6 +881,161 @@
         </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing10.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>114299</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>484984</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7F935630-28E1-48F6-4587-3CBDB04BA359}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="939799" y="9245600"/>
+          <a:ext cx="10276685" cy="1358900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>698500</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Straight Arrow Connector 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{570D9F7E-A15D-1B7B-9C91-6EBEAAB249BC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1524000" y="7061200"/>
+          <a:ext cx="1447800" cy="2997200"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>88900</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>177800</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="6" name="Straight Arrow Connector 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FEE67BB4-7F9D-BA0C-1B14-04044ACB45C2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="914400" y="7493000"/>
+          <a:ext cx="1739900" cy="2349500"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1822,6 +2020,541 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F8CFFC0-5591-644E-9D64-38C71A58EE3F}">
+  <dimension ref="A4:N53"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="L31" sqref="L31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="3"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B6" s="4"/>
+      <c r="C6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" s="5"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B7" s="4"/>
+      <c r="D7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7" s="5"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B8" s="4"/>
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" s="5"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B9" s="4"/>
+      <c r="D9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F9" s="5"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B10" s="4"/>
+      <c r="D10" t="s">
+        <v>48</v>
+      </c>
+      <c r="F10" s="5"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B11" s="4"/>
+      <c r="D11" t="s">
+        <v>49</v>
+      </c>
+      <c r="F11" s="5"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B12" s="4"/>
+      <c r="D12" t="s">
+        <v>120</v>
+      </c>
+      <c r="F12" s="5"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B13" s="4"/>
+      <c r="D13" t="s">
+        <v>128</v>
+      </c>
+      <c r="F13" s="5"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B14" s="4"/>
+      <c r="D14" s="19" t="s">
+        <v>155</v>
+      </c>
+      <c r="F14" s="5"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B15" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F15" s="5"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B16" s="4"/>
+      <c r="C16" t="s">
+        <v>35</v>
+      </c>
+      <c r="F16" s="5"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B17" s="4"/>
+      <c r="C17" t="s">
+        <v>97</v>
+      </c>
+      <c r="F17" s="5"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B18" s="4"/>
+      <c r="C18" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="F18" s="5"/>
+      <c r="G18" t="s">
+        <v>13</v>
+      </c>
+      <c r="H18" s="17" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B19" s="6"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="8"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22" s="10" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B23" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="3"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B24" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="C24" s="20"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="20"/>
+      <c r="H24" s="20"/>
+      <c r="I24" s="20"/>
+      <c r="J24" s="5"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B25" s="4"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="20"/>
+      <c r="H25" s="20"/>
+      <c r="I25" s="20"/>
+      <c r="J25" s="5"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B26" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="C26" s="20"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="20"/>
+      <c r="H26" s="20"/>
+      <c r="I26" s="20"/>
+      <c r="J26" s="5"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B27" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C27" s="20"/>
+      <c r="D27" s="20"/>
+      <c r="E27" s="20"/>
+      <c r="F27" s="20"/>
+      <c r="G27" s="20"/>
+      <c r="H27" s="20"/>
+      <c r="I27" s="20"/>
+      <c r="J27" s="5"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B28" s="4"/>
+      <c r="C28" s="20"/>
+      <c r="D28" s="20"/>
+      <c r="E28" s="20"/>
+      <c r="F28" s="20"/>
+      <c r="G28" s="20"/>
+      <c r="H28" s="20"/>
+      <c r="I28" s="20"/>
+      <c r="J28" s="5"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B29" s="4"/>
+      <c r="C29" s="20"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="20"/>
+      <c r="F29" s="20"/>
+      <c r="G29" s="20"/>
+      <c r="H29" s="20"/>
+      <c r="I29" s="20"/>
+      <c r="J29" s="5"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B30" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="C30" s="20"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="20"/>
+      <c r="J30" s="5"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B31" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="C31" s="20"/>
+      <c r="D31" s="20"/>
+      <c r="E31" s="20"/>
+      <c r="F31" s="20"/>
+      <c r="G31" s="20"/>
+      <c r="H31" s="20"/>
+      <c r="I31" s="20"/>
+      <c r="J31" s="5"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B32" s="4"/>
+      <c r="C32" s="20"/>
+      <c r="D32" s="20"/>
+      <c r="E32" s="20"/>
+      <c r="F32" s="20"/>
+      <c r="G32" s="20"/>
+      <c r="H32" s="20"/>
+      <c r="I32" s="20"/>
+      <c r="J32" s="5"/>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B33" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="C33" s="20"/>
+      <c r="D33" s="20"/>
+      <c r="E33" s="20"/>
+      <c r="F33" s="20"/>
+      <c r="G33" s="20"/>
+      <c r="H33" s="20"/>
+      <c r="I33" s="20"/>
+      <c r="J33" s="5"/>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B34" s="4"/>
+      <c r="C34" s="20"/>
+      <c r="D34" s="20"/>
+      <c r="E34" s="20"/>
+      <c r="F34" s="20"/>
+      <c r="G34" s="20"/>
+      <c r="H34" s="20"/>
+      <c r="I34" s="20"/>
+      <c r="J34" s="5"/>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B35" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="C35" s="20"/>
+      <c r="D35" s="20"/>
+      <c r="E35" s="20"/>
+      <c r="F35" s="20"/>
+      <c r="G35" s="20"/>
+      <c r="H35" s="20"/>
+      <c r="I35" s="20"/>
+      <c r="J35" s="5"/>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B36" s="4"/>
+      <c r="C36" s="20"/>
+      <c r="D36" s="20"/>
+      <c r="E36" s="20"/>
+      <c r="F36" s="20"/>
+      <c r="G36" s="20"/>
+      <c r="H36" s="20"/>
+      <c r="I36" s="20"/>
+      <c r="J36" s="5"/>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B37" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="C37" s="20"/>
+      <c r="D37" s="20"/>
+      <c r="E37" s="20"/>
+      <c r="F37" s="20"/>
+      <c r="G37" s="20"/>
+      <c r="H37" s="20"/>
+      <c r="I37" s="20"/>
+      <c r="J37" s="5"/>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B38" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="C38" s="20"/>
+      <c r="D38" s="20"/>
+      <c r="E38" s="20"/>
+      <c r="F38" s="20"/>
+      <c r="G38" s="20"/>
+      <c r="H38" s="20"/>
+      <c r="I38" s="20"/>
+      <c r="J38" s="5"/>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B39" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="C39" s="20"/>
+      <c r="D39" s="20"/>
+      <c r="E39" s="20"/>
+      <c r="F39" s="20"/>
+      <c r="G39" s="20"/>
+      <c r="H39" s="20"/>
+      <c r="I39" s="20"/>
+      <c r="J39" s="5"/>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B40" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C40" s="20"/>
+      <c r="D40" s="20"/>
+      <c r="E40" s="20"/>
+      <c r="F40" s="20"/>
+      <c r="G40" s="20"/>
+      <c r="H40" s="20"/>
+      <c r="I40" s="20"/>
+      <c r="J40" s="5"/>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B41" s="6"/>
+      <c r="C41" s="7"/>
+      <c r="D41" s="7"/>
+      <c r="E41" s="7"/>
+      <c r="F41" s="7"/>
+      <c r="G41" s="7"/>
+      <c r="H41" s="7"/>
+      <c r="I41" s="7"/>
+      <c r="J41" s="8"/>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A44" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B44" s="2"/>
+      <c r="C44" s="2"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
+      <c r="F44" s="2"/>
+      <c r="G44" s="2"/>
+      <c r="H44" s="2"/>
+      <c r="I44" s="2"/>
+      <c r="J44" s="2"/>
+      <c r="K44" s="2"/>
+      <c r="L44" s="2"/>
+      <c r="M44" s="2"/>
+      <c r="N44" s="3"/>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A45" s="4"/>
+      <c r="B45" s="20" t="s">
+        <v>181</v>
+      </c>
+      <c r="C45" s="20"/>
+      <c r="D45" s="20"/>
+      <c r="E45" s="20"/>
+      <c r="F45" s="20"/>
+      <c r="G45" s="20"/>
+      <c r="H45" s="20"/>
+      <c r="I45" s="20"/>
+      <c r="J45" s="20"/>
+      <c r="K45" s="20"/>
+      <c r="L45" s="20"/>
+      <c r="M45" s="20"/>
+      <c r="N45" s="5"/>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A46" s="4"/>
+      <c r="B46" s="20"/>
+      <c r="C46" s="20"/>
+      <c r="D46" s="20"/>
+      <c r="E46" s="20"/>
+      <c r="F46" s="20"/>
+      <c r="G46" s="20"/>
+      <c r="H46" s="20"/>
+      <c r="I46" s="20"/>
+      <c r="J46" s="20"/>
+      <c r="K46" s="20"/>
+      <c r="L46" s="20"/>
+      <c r="M46" s="20"/>
+      <c r="N46" s="5"/>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A47" s="4"/>
+      <c r="B47" s="20"/>
+      <c r="C47" s="20"/>
+      <c r="D47" s="20"/>
+      <c r="E47" s="20"/>
+      <c r="F47" s="20"/>
+      <c r="G47" s="20"/>
+      <c r="H47" s="20"/>
+      <c r="I47" s="20"/>
+      <c r="J47" s="20"/>
+      <c r="K47" s="20"/>
+      <c r="L47" s="20"/>
+      <c r="M47" s="20"/>
+      <c r="N47" s="5"/>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A48" s="4"/>
+      <c r="B48" s="20"/>
+      <c r="C48" s="20"/>
+      <c r="D48" s="20"/>
+      <c r="E48" s="20"/>
+      <c r="F48" s="20"/>
+      <c r="G48" s="20"/>
+      <c r="H48" s="20"/>
+      <c r="I48" s="20"/>
+      <c r="J48" s="20"/>
+      <c r="K48" s="20"/>
+      <c r="L48" s="20"/>
+      <c r="M48" s="20"/>
+      <c r="N48" s="5"/>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A49" s="4"/>
+      <c r="B49" s="20"/>
+      <c r="C49" s="20"/>
+      <c r="D49" s="20"/>
+      <c r="E49" s="20"/>
+      <c r="F49" s="20"/>
+      <c r="G49" s="20"/>
+      <c r="H49" s="20"/>
+      <c r="I49" s="20"/>
+      <c r="J49" s="20"/>
+      <c r="K49" s="20"/>
+      <c r="L49" s="20"/>
+      <c r="M49" s="20"/>
+      <c r="N49" s="5"/>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A50" s="4"/>
+      <c r="B50" s="20"/>
+      <c r="C50" s="20"/>
+      <c r="D50" s="20"/>
+      <c r="E50" s="20"/>
+      <c r="F50" s="20"/>
+      <c r="G50" s="20"/>
+      <c r="H50" s="20"/>
+      <c r="I50" s="20"/>
+      <c r="J50" s="20"/>
+      <c r="K50" s="20"/>
+      <c r="L50" s="20"/>
+      <c r="M50" s="20"/>
+      <c r="N50" s="5"/>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A51" s="4"/>
+      <c r="B51" s="20"/>
+      <c r="C51" s="20"/>
+      <c r="D51" s="20"/>
+      <c r="E51" s="20"/>
+      <c r="F51" s="20"/>
+      <c r="G51" s="20"/>
+      <c r="H51" s="20"/>
+      <c r="I51" s="20"/>
+      <c r="J51" s="20"/>
+      <c r="K51" s="20"/>
+      <c r="L51" s="20"/>
+      <c r="M51" s="20"/>
+      <c r="N51" s="5"/>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A52" s="4"/>
+      <c r="B52" s="20"/>
+      <c r="C52" s="20"/>
+      <c r="D52" s="20"/>
+      <c r="E52" s="20"/>
+      <c r="F52" s="20"/>
+      <c r="G52" s="20"/>
+      <c r="H52" s="20"/>
+      <c r="I52" s="20"/>
+      <c r="J52" s="20"/>
+      <c r="K52" s="20"/>
+      <c r="L52" s="20"/>
+      <c r="M52" s="20"/>
+      <c r="N52" s="5"/>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A53" s="6"/>
+      <c r="B53" s="7"/>
+      <c r="C53" s="7"/>
+      <c r="D53" s="7"/>
+      <c r="E53" s="7"/>
+      <c r="F53" s="7"/>
+      <c r="G53" s="7"/>
+      <c r="H53" s="7"/>
+      <c r="I53" s="7"/>
+      <c r="J53" s="7"/>
+      <c r="K53" s="7"/>
+      <c r="L53" s="7"/>
+      <c r="M53" s="7"/>
+      <c r="N53" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B0CC97E-5A37-2E41-A870-EAFA42883709}">
   <dimension ref="A4:O42"/>
@@ -4342,8 +5075,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EDE2FFD-E026-A448-8149-A1C2EFE66A1D}">
   <dimension ref="A4:R47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4413,7 +5146,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B13" s="4"/>
-      <c r="D13" s="18" t="s">
+      <c r="D13" t="s">
         <v>128</v>
       </c>
       <c r="F13" s="5"/>
@@ -4475,37 +5208,29 @@
       <c r="B23" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="C23" s="19"/>
-      <c r="D23" s="19"/>
       <c r="E23" s="5"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B24" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="C24" s="19"/>
-      <c r="D24" s="19"/>
       <c r="E24" s="5"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B25" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="C25" s="19"/>
-      <c r="D25" s="19"/>
       <c r="E25" s="5"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B26" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="C26" s="19"/>
-      <c r="D26" s="19"/>
       <c r="E26" s="5"/>
       <c r="F26" t="s">
         <v>13</v>
       </c>
-      <c r="G26" s="20" t="s">
+      <c r="G26" s="18" t="s">
         <v>167</v>
       </c>
     </row>
@@ -4513,16 +5238,12 @@
       <c r="B27" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="C27" s="19"/>
-      <c r="D27" s="19"/>
       <c r="E27" s="5"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B28" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="C28" s="19"/>
-      <c r="D28" s="19"/>
       <c r="E28" s="5"/>
       <c r="F28" t="s">
         <v>13</v>
@@ -4535,16 +5256,12 @@
       <c r="B29" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="C29" s="19"/>
-      <c r="D29" s="19"/>
       <c r="E29" s="5"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B30" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="C30" s="19"/>
-      <c r="D30" s="19"/>
       <c r="E30" s="5"/>
       <c r="F30" t="s">
         <v>13</v>
@@ -4557,8 +5274,6 @@
       <c r="B31" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="C31" s="19"/>
-      <c r="D31" s="19"/>
       <c r="E31" s="5"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
@@ -4591,224 +5306,49 @@
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A36" s="4"/>
-      <c r="B36" s="19" t="s">
+      <c r="B36" t="s">
         <v>163</v>
       </c>
-      <c r="C36" s="19"/>
-      <c r="D36" s="19"/>
-      <c r="E36" s="19"/>
-      <c r="F36" s="19"/>
-      <c r="G36" s="19"/>
-      <c r="H36" s="19"/>
-      <c r="I36" s="19"/>
-      <c r="J36" s="19"/>
-      <c r="K36" s="19"/>
-      <c r="L36" s="19"/>
-      <c r="M36" s="19"/>
-      <c r="N36" s="19"/>
-      <c r="O36" s="19"/>
-      <c r="P36" s="19"/>
-      <c r="Q36" s="19"/>
       <c r="R36" s="5"/>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A37" s="4"/>
-      <c r="B37" s="19"/>
-      <c r="C37" s="19"/>
-      <c r="D37" s="19"/>
-      <c r="E37" s="19"/>
-      <c r="F37" s="19"/>
-      <c r="G37" s="19"/>
-      <c r="H37" s="19"/>
-      <c r="I37" s="19"/>
-      <c r="J37" s="19"/>
-      <c r="K37" s="19"/>
-      <c r="L37" s="19"/>
-      <c r="M37" s="19"/>
-      <c r="N37" s="19"/>
-      <c r="O37" s="19"/>
-      <c r="P37" s="19"/>
-      <c r="Q37" s="19"/>
       <c r="R37" s="5"/>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A38" s="4"/>
-      <c r="B38" s="19"/>
-      <c r="C38" s="19"/>
-      <c r="D38" s="19"/>
-      <c r="E38" s="19"/>
-      <c r="F38" s="19"/>
-      <c r="G38" s="19"/>
-      <c r="H38" s="19"/>
-      <c r="I38" s="19"/>
-      <c r="J38" s="19"/>
-      <c r="K38" s="19"/>
-      <c r="L38" s="19"/>
-      <c r="M38" s="19"/>
-      <c r="N38" s="19"/>
-      <c r="O38" s="19"/>
-      <c r="P38" s="19"/>
-      <c r="Q38" s="19"/>
       <c r="R38" s="5"/>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A39" s="4"/>
-      <c r="B39" s="19"/>
-      <c r="C39" s="19"/>
-      <c r="D39" s="19"/>
-      <c r="E39" s="19"/>
-      <c r="F39" s="19"/>
-      <c r="G39" s="19"/>
-      <c r="H39" s="19"/>
-      <c r="I39" s="19"/>
-      <c r="J39" s="19"/>
-      <c r="K39" s="19"/>
-      <c r="L39" s="19"/>
-      <c r="M39" s="19"/>
-      <c r="N39" s="19"/>
-      <c r="O39" s="19"/>
-      <c r="P39" s="19"/>
-      <c r="Q39" s="19"/>
       <c r="R39" s="5"/>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A40" s="4"/>
-      <c r="B40" s="19"/>
-      <c r="C40" s="19"/>
-      <c r="D40" s="19"/>
-      <c r="E40" s="19"/>
-      <c r="F40" s="19"/>
-      <c r="G40" s="19"/>
-      <c r="H40" s="19"/>
-      <c r="I40" s="19"/>
-      <c r="J40" s="19"/>
-      <c r="K40" s="19"/>
-      <c r="L40" s="19"/>
-      <c r="M40" s="19"/>
-      <c r="N40" s="19"/>
-      <c r="O40" s="19"/>
-      <c r="P40" s="19"/>
-      <c r="Q40" s="19"/>
       <c r="R40" s="5"/>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A41" s="4"/>
-      <c r="B41" s="19"/>
-      <c r="C41" s="19"/>
-      <c r="D41" s="19"/>
-      <c r="E41" s="19"/>
-      <c r="F41" s="19"/>
-      <c r="G41" s="19"/>
-      <c r="H41" s="19"/>
-      <c r="I41" s="19"/>
-      <c r="J41" s="19"/>
-      <c r="K41" s="19"/>
-      <c r="L41" s="19"/>
-      <c r="M41" s="19"/>
-      <c r="N41" s="19"/>
-      <c r="O41" s="19"/>
-      <c r="P41" s="19"/>
-      <c r="Q41" s="19"/>
       <c r="R41" s="5"/>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A42" s="4"/>
-      <c r="B42" s="19"/>
-      <c r="C42" s="19"/>
-      <c r="D42" s="19"/>
-      <c r="E42" s="19"/>
-      <c r="F42" s="19"/>
-      <c r="G42" s="19"/>
-      <c r="H42" s="19"/>
-      <c r="I42" s="19"/>
-      <c r="J42" s="19"/>
-      <c r="K42" s="19"/>
-      <c r="L42" s="19"/>
-      <c r="M42" s="19"/>
-      <c r="N42" s="19"/>
-      <c r="O42" s="19"/>
-      <c r="P42" s="19"/>
-      <c r="Q42" s="19"/>
       <c r="R42" s="5"/>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A43" s="4"/>
-      <c r="B43" s="19"/>
-      <c r="C43" s="19"/>
-      <c r="D43" s="19"/>
-      <c r="E43" s="19"/>
-      <c r="F43" s="19"/>
-      <c r="G43" s="19"/>
-      <c r="H43" s="19"/>
-      <c r="I43" s="19"/>
-      <c r="J43" s="19"/>
-      <c r="K43" s="19"/>
-      <c r="L43" s="19"/>
-      <c r="M43" s="19"/>
-      <c r="N43" s="19"/>
-      <c r="O43" s="19"/>
-      <c r="P43" s="19"/>
-      <c r="Q43" s="19"/>
       <c r="R43" s="5"/>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A44" s="4"/>
-      <c r="B44" s="19"/>
-      <c r="C44" s="19"/>
-      <c r="D44" s="19"/>
-      <c r="E44" s="19"/>
-      <c r="F44" s="19"/>
-      <c r="G44" s="19"/>
-      <c r="H44" s="19"/>
-      <c r="I44" s="19"/>
-      <c r="J44" s="19"/>
-      <c r="K44" s="19"/>
-      <c r="L44" s="19"/>
-      <c r="M44" s="19"/>
-      <c r="N44" s="19"/>
-      <c r="O44" s="19"/>
-      <c r="P44" s="19"/>
-      <c r="Q44" s="19"/>
       <c r="R44" s="5"/>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A45" s="4"/>
-      <c r="B45" s="19"/>
-      <c r="C45" s="19"/>
-      <c r="D45" s="19"/>
-      <c r="E45" s="19"/>
-      <c r="F45" s="19"/>
-      <c r="G45" s="19"/>
-      <c r="H45" s="19"/>
-      <c r="I45" s="19"/>
-      <c r="J45" s="19"/>
-      <c r="K45" s="19"/>
-      <c r="L45" s="19"/>
-      <c r="M45" s="19"/>
-      <c r="N45" s="19"/>
-      <c r="O45" s="19"/>
-      <c r="P45" s="19"/>
-      <c r="Q45" s="19"/>
       <c r="R45" s="5"/>
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A46" s="4"/>
-      <c r="B46" s="19"/>
-      <c r="C46" s="19"/>
-      <c r="D46" s="19"/>
-      <c r="E46" s="19"/>
-      <c r="F46" s="19"/>
-      <c r="G46" s="19"/>
-      <c r="H46" s="19"/>
-      <c r="I46" s="19"/>
-      <c r="J46" s="19"/>
-      <c r="K46" s="19"/>
-      <c r="L46" s="19"/>
-      <c r="M46" s="19"/>
-      <c r="N46" s="19"/>
-      <c r="O46" s="19"/>
-      <c r="P46" s="19"/>
-      <c r="Q46" s="19"/>
       <c r="R46" s="5"/>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Exe 04 - tag
</commit_message>
<xml_diff>
--- a/me/1.Lap-trinh-python/1.Lap-trinh-python/2.lam-viec-voi-cac-kieu-du-lieu.xlsx
+++ b/me/1.Lap-trinh-python/1.Lap-trinh-python/2.lam-viec-voi-cac-kieu-du-lieu.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vudinhquang/Documents/quang/python/me/1.Lap-trinh-python/1.Lap-trinh-python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A44A7B3-D1C2-E844-9FEB-E152DC4AFEE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F598E52C-2742-9F4C-ABB3-55E1FB03453F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1260" windowWidth="31460" windowHeight="18720" activeTab="9" xr2:uid="{FC6AE9BB-4BEF-564A-A974-1CE698055D30}"/>
+    <workbookView xWindow="1560" yWindow="1260" windowWidth="31460" windowHeight="18720" activeTab="10" xr2:uid="{FC6AE9BB-4BEF-564A-A974-1CE698055D30}"/>
   </bookViews>
   <sheets>
     <sheet name="Variable" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,7 @@
     <sheet name="String 04" sheetId="8" r:id="rId8"/>
     <sheet name="String 05" sheetId="9" r:id="rId9"/>
     <sheet name="Exe 03 - birthday" sheetId="10" r:id="rId10"/>
+    <sheet name="Exe 04 - tag" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="191">
   <si>
     <t>構成</t>
   </si>
@@ -650,6 +651,33 @@
   </si>
   <si>
     <t>python3 exe_03_birthday.py</t>
+  </si>
+  <si>
+    <t>exe_04_tag.py</t>
+  </si>
+  <si>
+    <t>python/exe/exe_04_tag.py</t>
+  </si>
+  <si>
+    <t># Input : Cho 1 chuỗi và tag html</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># Output: Tạo ra tag html với nội dung là chuỗi </t>
+  </si>
+  <si>
+    <t>content = "Hello"</t>
+  </si>
+  <si>
+    <t>tag     = "div"</t>
+  </si>
+  <si>
+    <t>result1  = "&lt;{tag}&gt;{content}&lt;/{tag}&gt;".format(tag = tag, content = content)</t>
+  </si>
+  <si>
+    <t>result2  = "&lt;%s&gt;%s&lt;/%s&gt;" % (tag, content, tag)</t>
+  </si>
+  <si>
+    <t>python3 exe_04_tag.py</t>
   </si>
 </sst>
 </file>
@@ -1036,6 +1064,55 @@
         </a:fontRef>
       </xdr:style>
     </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing11.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>88900</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>82820</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1A4DBA92-A127-A6FA-C0E5-52FF966A59EA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="914400" y="7594600"/>
+          <a:ext cx="11550920" cy="1409700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -2024,8 +2101,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F8CFFC0-5591-644E-9D64-38C71A58EE3F}">
   <dimension ref="A4:N53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="L31" sqref="L31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P29" sqref="P29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2102,7 +2179,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B14" s="4"/>
-      <c r="D14" s="19" t="s">
+      <c r="D14" t="s">
         <v>155</v>
       </c>
       <c r="F14" s="5"/>
@@ -2169,209 +2246,90 @@
       <c r="B24" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="C24" s="20"/>
-      <c r="D24" s="20"/>
-      <c r="E24" s="20"/>
-      <c r="F24" s="20"/>
-      <c r="G24" s="20"/>
-      <c r="H24" s="20"/>
-      <c r="I24" s="20"/>
       <c r="J24" s="5"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B25" s="4"/>
-      <c r="C25" s="20"/>
-      <c r="D25" s="20"/>
-      <c r="E25" s="20"/>
-      <c r="F25" s="20"/>
-      <c r="G25" s="20"/>
-      <c r="H25" s="20"/>
-      <c r="I25" s="20"/>
       <c r="J25" s="5"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B26" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="C26" s="20"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="20"/>
-      <c r="F26" s="20"/>
-      <c r="G26" s="20"/>
-      <c r="H26" s="20"/>
-      <c r="I26" s="20"/>
       <c r="J26" s="5"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B27" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="C27" s="20"/>
-      <c r="D27" s="20"/>
-      <c r="E27" s="20"/>
-      <c r="F27" s="20"/>
-      <c r="G27" s="20"/>
-      <c r="H27" s="20"/>
-      <c r="I27" s="20"/>
       <c r="J27" s="5"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B28" s="4"/>
-      <c r="C28" s="20"/>
-      <c r="D28" s="20"/>
-      <c r="E28" s="20"/>
-      <c r="F28" s="20"/>
-      <c r="G28" s="20"/>
-      <c r="H28" s="20"/>
-      <c r="I28" s="20"/>
       <c r="J28" s="5"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B29" s="4"/>
-      <c r="C29" s="20"/>
-      <c r="D29" s="20"/>
-      <c r="E29" s="20"/>
-      <c r="F29" s="20"/>
-      <c r="G29" s="20"/>
-      <c r="H29" s="20"/>
-      <c r="I29" s="20"/>
       <c r="J29" s="5"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B30" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="C30" s="20"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="20"/>
-      <c r="G30" s="20"/>
-      <c r="H30" s="20"/>
-      <c r="I30" s="20"/>
       <c r="J30" s="5"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B31" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="C31" s="20"/>
-      <c r="D31" s="20"/>
-      <c r="E31" s="20"/>
-      <c r="F31" s="20"/>
-      <c r="G31" s="20"/>
-      <c r="H31" s="20"/>
-      <c r="I31" s="20"/>
       <c r="J31" s="5"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B32" s="4"/>
-      <c r="C32" s="20"/>
-      <c r="D32" s="20"/>
-      <c r="E32" s="20"/>
-      <c r="F32" s="20"/>
-      <c r="G32" s="20"/>
-      <c r="H32" s="20"/>
-      <c r="I32" s="20"/>
       <c r="J32" s="5"/>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B33" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="C33" s="20"/>
-      <c r="D33" s="20"/>
-      <c r="E33" s="20"/>
-      <c r="F33" s="20"/>
-      <c r="G33" s="20"/>
-      <c r="H33" s="20"/>
-      <c r="I33" s="20"/>
       <c r="J33" s="5"/>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B34" s="4"/>
-      <c r="C34" s="20"/>
-      <c r="D34" s="20"/>
-      <c r="E34" s="20"/>
-      <c r="F34" s="20"/>
-      <c r="G34" s="20"/>
-      <c r="H34" s="20"/>
-      <c r="I34" s="20"/>
       <c r="J34" s="5"/>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B35" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="C35" s="20"/>
-      <c r="D35" s="20"/>
-      <c r="E35" s="20"/>
-      <c r="F35" s="20"/>
-      <c r="G35" s="20"/>
-      <c r="H35" s="20"/>
-      <c r="I35" s="20"/>
       <c r="J35" s="5"/>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B36" s="4"/>
-      <c r="C36" s="20"/>
-      <c r="D36" s="20"/>
-      <c r="E36" s="20"/>
-      <c r="F36" s="20"/>
-      <c r="G36" s="20"/>
-      <c r="H36" s="20"/>
-      <c r="I36" s="20"/>
       <c r="J36" s="5"/>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B37" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="C37" s="20"/>
-      <c r="D37" s="20"/>
-      <c r="E37" s="20"/>
-      <c r="F37" s="20"/>
-      <c r="G37" s="20"/>
-      <c r="H37" s="20"/>
-      <c r="I37" s="20"/>
       <c r="J37" s="5"/>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B38" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="C38" s="20"/>
-      <c r="D38" s="20"/>
-      <c r="E38" s="20"/>
-      <c r="F38" s="20"/>
-      <c r="G38" s="20"/>
-      <c r="H38" s="20"/>
-      <c r="I38" s="20"/>
       <c r="J38" s="5"/>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B39" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="C39" s="20"/>
-      <c r="D39" s="20"/>
-      <c r="E39" s="20"/>
-      <c r="F39" s="20"/>
-      <c r="G39" s="20"/>
-      <c r="H39" s="20"/>
-      <c r="I39" s="20"/>
       <c r="J39" s="5"/>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B40" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C40" s="20"/>
-      <c r="D40" s="20"/>
-      <c r="E40" s="20"/>
-      <c r="F40" s="20"/>
-      <c r="G40" s="20"/>
-      <c r="H40" s="20"/>
-      <c r="I40" s="20"/>
       <c r="J40" s="5"/>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.2">
@@ -2405,132 +2363,37 @@
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A45" s="4"/>
-      <c r="B45" s="20" t="s">
+      <c r="B45" t="s">
         <v>181</v>
       </c>
-      <c r="C45" s="20"/>
-      <c r="D45" s="20"/>
-      <c r="E45" s="20"/>
-      <c r="F45" s="20"/>
-      <c r="G45" s="20"/>
-      <c r="H45" s="20"/>
-      <c r="I45" s="20"/>
-      <c r="J45" s="20"/>
-      <c r="K45" s="20"/>
-      <c r="L45" s="20"/>
-      <c r="M45" s="20"/>
       <c r="N45" s="5"/>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A46" s="4"/>
-      <c r="B46" s="20"/>
-      <c r="C46" s="20"/>
-      <c r="D46" s="20"/>
-      <c r="E46" s="20"/>
-      <c r="F46" s="20"/>
-      <c r="G46" s="20"/>
-      <c r="H46" s="20"/>
-      <c r="I46" s="20"/>
-      <c r="J46" s="20"/>
-      <c r="K46" s="20"/>
-      <c r="L46" s="20"/>
-      <c r="M46" s="20"/>
       <c r="N46" s="5"/>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A47" s="4"/>
-      <c r="B47" s="20"/>
-      <c r="C47" s="20"/>
-      <c r="D47" s="20"/>
-      <c r="E47" s="20"/>
-      <c r="F47" s="20"/>
-      <c r="G47" s="20"/>
-      <c r="H47" s="20"/>
-      <c r="I47" s="20"/>
-      <c r="J47" s="20"/>
-      <c r="K47" s="20"/>
-      <c r="L47" s="20"/>
-      <c r="M47" s="20"/>
       <c r="N47" s="5"/>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A48" s="4"/>
-      <c r="B48" s="20"/>
-      <c r="C48" s="20"/>
-      <c r="D48" s="20"/>
-      <c r="E48" s="20"/>
-      <c r="F48" s="20"/>
-      <c r="G48" s="20"/>
-      <c r="H48" s="20"/>
-      <c r="I48" s="20"/>
-      <c r="J48" s="20"/>
-      <c r="K48" s="20"/>
-      <c r="L48" s="20"/>
-      <c r="M48" s="20"/>
       <c r="N48" s="5"/>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A49" s="4"/>
-      <c r="B49" s="20"/>
-      <c r="C49" s="20"/>
-      <c r="D49" s="20"/>
-      <c r="E49" s="20"/>
-      <c r="F49" s="20"/>
-      <c r="G49" s="20"/>
-      <c r="H49" s="20"/>
-      <c r="I49" s="20"/>
-      <c r="J49" s="20"/>
-      <c r="K49" s="20"/>
-      <c r="L49" s="20"/>
-      <c r="M49" s="20"/>
       <c r="N49" s="5"/>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A50" s="4"/>
-      <c r="B50" s="20"/>
-      <c r="C50" s="20"/>
-      <c r="D50" s="20"/>
-      <c r="E50" s="20"/>
-      <c r="F50" s="20"/>
-      <c r="G50" s="20"/>
-      <c r="H50" s="20"/>
-      <c r="I50" s="20"/>
-      <c r="J50" s="20"/>
-      <c r="K50" s="20"/>
-      <c r="L50" s="20"/>
-      <c r="M50" s="20"/>
       <c r="N50" s="5"/>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A51" s="4"/>
-      <c r="B51" s="20"/>
-      <c r="C51" s="20"/>
-      <c r="D51" s="20"/>
-      <c r="E51" s="20"/>
-      <c r="F51" s="20"/>
-      <c r="G51" s="20"/>
-      <c r="H51" s="20"/>
-      <c r="I51" s="20"/>
-      <c r="J51" s="20"/>
-      <c r="K51" s="20"/>
-      <c r="L51" s="20"/>
-      <c r="M51" s="20"/>
       <c r="N51" s="5"/>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A52" s="4"/>
-      <c r="B52" s="20"/>
-      <c r="C52" s="20"/>
-      <c r="D52" s="20"/>
-      <c r="E52" s="20"/>
-      <c r="F52" s="20"/>
-      <c r="G52" s="20"/>
-      <c r="H52" s="20"/>
-      <c r="I52" s="20"/>
-      <c r="J52" s="20"/>
-      <c r="K52" s="20"/>
-      <c r="L52" s="20"/>
-      <c r="M52" s="20"/>
       <c r="N52" s="5"/>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.2">
@@ -2548,6 +2411,433 @@
       <c r="L53" s="7"/>
       <c r="M53" s="7"/>
       <c r="N53" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3056AB1-F460-8745-99A9-DE6A744B9F62}">
+  <dimension ref="A4:P45"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="M54" sqref="M54"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="3"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B6" s="4"/>
+      <c r="C6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" s="5"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B7" s="4"/>
+      <c r="D7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7" s="5"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B8" s="4"/>
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" s="5"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B9" s="4"/>
+      <c r="D9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F9" s="5"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B10" s="4"/>
+      <c r="D10" t="s">
+        <v>48</v>
+      </c>
+      <c r="F10" s="5"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B11" s="4"/>
+      <c r="D11" t="s">
+        <v>49</v>
+      </c>
+      <c r="F11" s="5"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B12" s="4"/>
+      <c r="D12" t="s">
+        <v>120</v>
+      </c>
+      <c r="F12" s="5"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B13" s="4"/>
+      <c r="D13" t="s">
+        <v>128</v>
+      </c>
+      <c r="F13" s="5"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B14" s="4"/>
+      <c r="D14" t="s">
+        <v>155</v>
+      </c>
+      <c r="F14" s="5"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B15" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F15" s="5"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B16" s="4"/>
+      <c r="C16" t="s">
+        <v>35</v>
+      </c>
+      <c r="F16" s="5"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B17" s="4"/>
+      <c r="C17" t="s">
+        <v>97</v>
+      </c>
+      <c r="F17" s="5"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B18" s="4"/>
+      <c r="C18" s="19" t="s">
+        <v>168</v>
+      </c>
+      <c r="F18" s="5"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B19" s="4"/>
+      <c r="C19" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="F19" s="5"/>
+      <c r="G19" t="s">
+        <v>13</v>
+      </c>
+      <c r="H19" s="17" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B20" s="6"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="8"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" s="10" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B24" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="3"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B25" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="C25" s="20"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="5"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B26" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C26" s="20"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="5"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B27" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C27" s="20"/>
+      <c r="D27" s="20"/>
+      <c r="E27" s="20"/>
+      <c r="F27" s="20"/>
+      <c r="G27" s="5"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B28" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="C28" s="20"/>
+      <c r="D28" s="20"/>
+      <c r="E28" s="20"/>
+      <c r="F28" s="20"/>
+      <c r="G28" s="5"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B29" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="C29" s="20"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="20"/>
+      <c r="F29" s="20"/>
+      <c r="G29" s="5"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B30" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C30" s="20"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="5"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B31" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C31" s="20"/>
+      <c r="D31" s="20"/>
+      <c r="E31" s="20"/>
+      <c r="F31" s="20"/>
+      <c r="G31" s="5"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B32" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C32" s="20"/>
+      <c r="D32" s="20"/>
+      <c r="E32" s="20"/>
+      <c r="F32" s="20"/>
+      <c r="G32" s="5"/>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B33" s="6"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
+      <c r="G33" s="8"/>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A36" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="2"/>
+      <c r="J36" s="2"/>
+      <c r="K36" s="2"/>
+      <c r="L36" s="2"/>
+      <c r="M36" s="2"/>
+      <c r="N36" s="2"/>
+      <c r="O36" s="2"/>
+      <c r="P36" s="3"/>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A37" s="4"/>
+      <c r="B37" s="20" t="s">
+        <v>190</v>
+      </c>
+      <c r="C37" s="20"/>
+      <c r="D37" s="20"/>
+      <c r="E37" s="20"/>
+      <c r="F37" s="20"/>
+      <c r="G37" s="20"/>
+      <c r="H37" s="20"/>
+      <c r="I37" s="20"/>
+      <c r="J37" s="20"/>
+      <c r="K37" s="20"/>
+      <c r="L37" s="20"/>
+      <c r="M37" s="20"/>
+      <c r="N37" s="20"/>
+      <c r="O37" s="20"/>
+      <c r="P37" s="5"/>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A38" s="4"/>
+      <c r="B38" s="20"/>
+      <c r="C38" s="20"/>
+      <c r="D38" s="20"/>
+      <c r="E38" s="20"/>
+      <c r="F38" s="20"/>
+      <c r="G38" s="20"/>
+      <c r="H38" s="20"/>
+      <c r="I38" s="20"/>
+      <c r="J38" s="20"/>
+      <c r="K38" s="20"/>
+      <c r="L38" s="20"/>
+      <c r="M38" s="20"/>
+      <c r="N38" s="20"/>
+      <c r="O38" s="20"/>
+      <c r="P38" s="5"/>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A39" s="4"/>
+      <c r="B39" s="20"/>
+      <c r="C39" s="20"/>
+      <c r="D39" s="20"/>
+      <c r="E39" s="20"/>
+      <c r="F39" s="20"/>
+      <c r="G39" s="20"/>
+      <c r="H39" s="20"/>
+      <c r="I39" s="20"/>
+      <c r="J39" s="20"/>
+      <c r="K39" s="20"/>
+      <c r="L39" s="20"/>
+      <c r="M39" s="20"/>
+      <c r="N39" s="20"/>
+      <c r="O39" s="20"/>
+      <c r="P39" s="5"/>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A40" s="4"/>
+      <c r="B40" s="20"/>
+      <c r="C40" s="20"/>
+      <c r="D40" s="20"/>
+      <c r="E40" s="20"/>
+      <c r="F40" s="20"/>
+      <c r="G40" s="20"/>
+      <c r="H40" s="20"/>
+      <c r="I40" s="20"/>
+      <c r="J40" s="20"/>
+      <c r="K40" s="20"/>
+      <c r="L40" s="20"/>
+      <c r="M40" s="20"/>
+      <c r="N40" s="20"/>
+      <c r="O40" s="20"/>
+      <c r="P40" s="5"/>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A41" s="4"/>
+      <c r="B41" s="20"/>
+      <c r="C41" s="20"/>
+      <c r="D41" s="20"/>
+      <c r="E41" s="20"/>
+      <c r="F41" s="20"/>
+      <c r="G41" s="20"/>
+      <c r="H41" s="20"/>
+      <c r="I41" s="20"/>
+      <c r="J41" s="20"/>
+      <c r="K41" s="20"/>
+      <c r="L41" s="20"/>
+      <c r="M41" s="20"/>
+      <c r="N41" s="20"/>
+      <c r="O41" s="20"/>
+      <c r="P41" s="5"/>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A42" s="4"/>
+      <c r="B42" s="20"/>
+      <c r="C42" s="20"/>
+      <c r="D42" s="20"/>
+      <c r="E42" s="20"/>
+      <c r="F42" s="20"/>
+      <c r="G42" s="20"/>
+      <c r="H42" s="20"/>
+      <c r="I42" s="20"/>
+      <c r="J42" s="20"/>
+      <c r="K42" s="20"/>
+      <c r="L42" s="20"/>
+      <c r="M42" s="20"/>
+      <c r="N42" s="20"/>
+      <c r="O42" s="20"/>
+      <c r="P42" s="5"/>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A43" s="4"/>
+      <c r="B43" s="20"/>
+      <c r="C43" s="20"/>
+      <c r="D43" s="20"/>
+      <c r="E43" s="20"/>
+      <c r="F43" s="20"/>
+      <c r="G43" s="20"/>
+      <c r="H43" s="20"/>
+      <c r="I43" s="20"/>
+      <c r="J43" s="20"/>
+      <c r="K43" s="20"/>
+      <c r="L43" s="20"/>
+      <c r="M43" s="20"/>
+      <c r="N43" s="20"/>
+      <c r="O43" s="20"/>
+      <c r="P43" s="5"/>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A44" s="4"/>
+      <c r="B44" s="20"/>
+      <c r="C44" s="20"/>
+      <c r="D44" s="20"/>
+      <c r="E44" s="20"/>
+      <c r="F44" s="20"/>
+      <c r="G44" s="20"/>
+      <c r="H44" s="20"/>
+      <c r="I44" s="20"/>
+      <c r="J44" s="20"/>
+      <c r="K44" s="20"/>
+      <c r="L44" s="20"/>
+      <c r="M44" s="20"/>
+      <c r="N44" s="20"/>
+      <c r="O44" s="20"/>
+      <c r="P44" s="5"/>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A45" s="6"/>
+      <c r="B45" s="7"/>
+      <c r="C45" s="7"/>
+      <c r="D45" s="7"/>
+      <c r="E45" s="7"/>
+      <c r="F45" s="7"/>
+      <c r="G45" s="7"/>
+      <c r="H45" s="7"/>
+      <c r="I45" s="7"/>
+      <c r="J45" s="7"/>
+      <c r="K45" s="7"/>
+      <c r="L45" s="7"/>
+      <c r="M45" s="7"/>
+      <c r="N45" s="7"/>
+      <c r="O45" s="7"/>
+      <c r="P45" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Exe 05 - extension
</commit_message>
<xml_diff>
--- a/me/1.Lap-trinh-python/1.Lap-trinh-python/2.lam-viec-voi-cac-kieu-du-lieu.xlsx
+++ b/me/1.Lap-trinh-python/1.Lap-trinh-python/2.lam-viec-voi-cac-kieu-du-lieu.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vudinhquang/Documents/quang/python/me/1.Lap-trinh-python/1.Lap-trinh-python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AB313A6-7CA2-E24A-9AA8-3D0EF14166E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{961B83AE-59C4-CA4D-9A47-A627CFD1FBBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1260" windowWidth="31460" windowHeight="18720" activeTab="14" xr2:uid="{FC6AE9BB-4BEF-564A-A974-1CE698055D30}"/>
+    <workbookView xWindow="1560" yWindow="1260" windowWidth="31460" windowHeight="18720" firstSheet="1" activeTab="15" xr2:uid="{FC6AE9BB-4BEF-564A-A974-1CE698055D30}"/>
   </bookViews>
   <sheets>
     <sheet name="Variable" sheetId="1" r:id="rId1"/>
@@ -28,6 +28,7 @@
     <sheet name="List 02" sheetId="13" r:id="rId13"/>
     <sheet name="List 03" sheetId="14" r:id="rId14"/>
     <sheet name="List 04" sheetId="15" r:id="rId15"/>
+    <sheet name="Exe 05 - extension" sheetId="16" r:id="rId16"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -49,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="281">
   <si>
     <t>構成</t>
   </si>
@@ -910,6 +911,48 @@
   </si>
   <si>
     <t>python3 04_list_03.py</t>
+  </si>
+  <si>
+    <t>exe_05_extension.py</t>
+  </si>
+  <si>
+    <t>quang/python/exe/exe_05_extension.py</t>
+  </si>
+  <si>
+    <t># Input     : Nhập vào tên tập tin</t>
+  </si>
+  <si>
+    <t># Output    : In ra phần mở rộng của tập tin</t>
+  </si>
+  <si>
+    <t>fileName    = input("Nhập vào tên tập tin: ")</t>
+  </si>
+  <si>
+    <t>fileExt     = fileName.split(".")</t>
+  </si>
+  <si>
+    <t>tmp         = len(fileExt)</t>
+  </si>
+  <si>
+    <t>result      = "Không xác định"</t>
+  </si>
+  <si>
+    <t>if(tmp &gt; 1):</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      result = fileExt[tmp - 1]</t>
+  </si>
+  <si>
+    <t>print("Phần mở rộng của tập tin: " + result)</t>
+  </si>
+  <si>
+    <t>①Không có phần mở rộng</t>
+  </si>
+  <si>
+    <t>python3 exe_05_extension.py</t>
+  </si>
+  <si>
+    <t>②Có phần mở rộng</t>
   </si>
 </sst>
 </file>
@@ -1758,6 +1801,205 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing16.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>114299</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>340366</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4049468A-5A38-D458-B41E-2AA2D7DBEE85}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="939799" y="9232900"/>
+          <a:ext cx="13434067" cy="1562100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>546100</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Straight Arrow Connector 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9989C76A-ED32-42C1-E750-CD4237FF0FE9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1371600" y="8915400"/>
+          <a:ext cx="1866900" cy="1143000"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>139699</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>365766</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6E076BCF-E11C-81AB-B929-501BF8B23401}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="965199" y="11912600"/>
+          <a:ext cx="13434067" cy="1562100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>355600</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>431800</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="Straight Arrow Connector 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E13FA4C9-16FB-9B6B-6517-A033416D7151}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1181100" y="11544300"/>
+          <a:ext cx="2552700" cy="1206500"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
@@ -3697,8 +3939,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1B88326-E0CC-2B43-9603-A438B4B4D264}">
   <dimension ref="A3:R93"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:H20"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="O34" sqref="O34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4321,8 +4563,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CF2E8D6-BD95-8B4A-98F3-1AE346C91BC2}">
   <dimension ref="A3:S66"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S33" sqref="S33"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4421,7 +4663,7 @@
         <v>13</v>
       </c>
       <c r="H15" s="17" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
@@ -4796,8 +5038,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F45AA01B-355C-D240-A407-8CAB748FE57B}">
   <dimension ref="A3:Q44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="J27" sqref="J27"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4888,7 +5130,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B15" s="4"/>
-      <c r="D15" s="19" t="s">
+      <c r="D15" t="s">
         <v>236</v>
       </c>
       <c r="F15" s="5"/>
@@ -4903,7 +5145,7 @@
         <v>13</v>
       </c>
       <c r="H16" s="17" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -4961,14 +5203,12 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B27" s="4"/>
-      <c r="C27" s="20"/>
       <c r="D27" s="5"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B28" s="4" t="s">
         <v>262</v>
       </c>
-      <c r="C28" s="20"/>
       <c r="D28" s="5"/>
       <c r="E28" t="s">
         <v>13</v>
@@ -4981,7 +5221,6 @@
       <c r="B29" s="4" t="s">
         <v>263</v>
       </c>
-      <c r="C29" s="20"/>
       <c r="D29" s="5"/>
       <c r="E29" t="s">
         <v>13</v>
@@ -4994,7 +5233,6 @@
       <c r="B30" s="4" t="s">
         <v>264</v>
       </c>
-      <c r="C30" s="20"/>
       <c r="D30" s="5"/>
       <c r="E30" t="s">
         <v>13</v>
@@ -5032,175 +5270,41 @@
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A35" s="4"/>
-      <c r="B35" s="20" t="s">
+      <c r="B35" t="s">
         <v>266</v>
       </c>
-      <c r="C35" s="20"/>
-      <c r="D35" s="20"/>
-      <c r="E35" s="20"/>
-      <c r="F35" s="20"/>
-      <c r="G35" s="20"/>
-      <c r="H35" s="20"/>
-      <c r="I35" s="20"/>
-      <c r="J35" s="20"/>
-      <c r="K35" s="20"/>
-      <c r="L35" s="20"/>
-      <c r="M35" s="20"/>
-      <c r="N35" s="20"/>
-      <c r="O35" s="20"/>
-      <c r="P35" s="20"/>
       <c r="Q35" s="5"/>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A36" s="4"/>
-      <c r="B36" s="20"/>
-      <c r="C36" s="20"/>
-      <c r="D36" s="20"/>
-      <c r="E36" s="20"/>
-      <c r="F36" s="20"/>
-      <c r="G36" s="20"/>
-      <c r="H36" s="20"/>
-      <c r="I36" s="20"/>
-      <c r="J36" s="20"/>
-      <c r="K36" s="20"/>
-      <c r="L36" s="20"/>
-      <c r="M36" s="20"/>
-      <c r="N36" s="20"/>
-      <c r="O36" s="20"/>
-      <c r="P36" s="20"/>
       <c r="Q36" s="5"/>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A37" s="4"/>
-      <c r="B37" s="20"/>
-      <c r="C37" s="20"/>
-      <c r="D37" s="20"/>
-      <c r="E37" s="20"/>
-      <c r="F37" s="20"/>
-      <c r="G37" s="20"/>
-      <c r="H37" s="20"/>
-      <c r="I37" s="20"/>
-      <c r="J37" s="20"/>
-      <c r="K37" s="20"/>
-      <c r="L37" s="20"/>
-      <c r="M37" s="20"/>
-      <c r="N37" s="20"/>
-      <c r="O37" s="20"/>
-      <c r="P37" s="20"/>
       <c r="Q37" s="5"/>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A38" s="4"/>
-      <c r="B38" s="20"/>
-      <c r="C38" s="20"/>
-      <c r="D38" s="20"/>
-      <c r="E38" s="20"/>
-      <c r="F38" s="20"/>
-      <c r="G38" s="20"/>
-      <c r="H38" s="20"/>
-      <c r="I38" s="20"/>
-      <c r="J38" s="20"/>
-      <c r="K38" s="20"/>
-      <c r="L38" s="20"/>
-      <c r="M38" s="20"/>
-      <c r="N38" s="20"/>
-      <c r="O38" s="20"/>
-      <c r="P38" s="20"/>
       <c r="Q38" s="5"/>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A39" s="4"/>
-      <c r="B39" s="20"/>
-      <c r="C39" s="20"/>
-      <c r="D39" s="20"/>
-      <c r="E39" s="20"/>
-      <c r="F39" s="20"/>
-      <c r="G39" s="20"/>
-      <c r="H39" s="20"/>
-      <c r="I39" s="20"/>
-      <c r="J39" s="20"/>
-      <c r="K39" s="20"/>
-      <c r="L39" s="20"/>
-      <c r="M39" s="20"/>
-      <c r="N39" s="20"/>
-      <c r="O39" s="20"/>
-      <c r="P39" s="20"/>
       <c r="Q39" s="5"/>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A40" s="4"/>
-      <c r="B40" s="20"/>
-      <c r="C40" s="20"/>
-      <c r="D40" s="20"/>
-      <c r="E40" s="20"/>
-      <c r="F40" s="20"/>
-      <c r="G40" s="20"/>
-      <c r="H40" s="20"/>
-      <c r="I40" s="20"/>
-      <c r="J40" s="20"/>
-      <c r="K40" s="20"/>
-      <c r="L40" s="20"/>
-      <c r="M40" s="20"/>
-      <c r="N40" s="20"/>
-      <c r="O40" s="20"/>
-      <c r="P40" s="20"/>
       <c r="Q40" s="5"/>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A41" s="4"/>
-      <c r="B41" s="20"/>
-      <c r="C41" s="20"/>
-      <c r="D41" s="20"/>
-      <c r="E41" s="20"/>
-      <c r="F41" s="20"/>
-      <c r="G41" s="20"/>
-      <c r="H41" s="20"/>
-      <c r="I41" s="20"/>
-      <c r="J41" s="20"/>
-      <c r="K41" s="20"/>
-      <c r="L41" s="20"/>
-      <c r="M41" s="20"/>
-      <c r="N41" s="20"/>
-      <c r="O41" s="20"/>
-      <c r="P41" s="20"/>
       <c r="Q41" s="5"/>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A42" s="4"/>
-      <c r="B42" s="20"/>
-      <c r="C42" s="20"/>
-      <c r="D42" s="20"/>
-      <c r="E42" s="20"/>
-      <c r="F42" s="20"/>
-      <c r="G42" s="20"/>
-      <c r="H42" s="20"/>
-      <c r="I42" s="20"/>
-      <c r="J42" s="20"/>
-      <c r="K42" s="20"/>
-      <c r="L42" s="20"/>
-      <c r="M42" s="20"/>
-      <c r="N42" s="20"/>
-      <c r="O42" s="20"/>
-      <c r="P42" s="20"/>
       <c r="Q42" s="5"/>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A43" s="4"/>
-      <c r="B43" s="20"/>
-      <c r="C43" s="20"/>
-      <c r="D43" s="20"/>
-      <c r="E43" s="20"/>
-      <c r="F43" s="20"/>
-      <c r="G43" s="20"/>
-      <c r="H43" s="20"/>
-      <c r="I43" s="20"/>
-      <c r="J43" s="20"/>
-      <c r="K43" s="20"/>
-      <c r="L43" s="20"/>
-      <c r="M43" s="20"/>
-      <c r="N43" s="20"/>
-      <c r="O43" s="20"/>
-      <c r="P43" s="20"/>
       <c r="Q43" s="5"/>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.2">
@@ -5221,6 +5325,838 @@
       <c r="O44" s="7"/>
       <c r="P44" s="7"/>
       <c r="Q44" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A712A9B9-9966-754B-ACEE-8BDB0475ACB2}">
+  <dimension ref="A3:S68"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="F74" sqref="F74"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="3"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B5" s="4"/>
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="5"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B6" s="4"/>
+      <c r="D6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" s="5"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B7" s="4"/>
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" s="5"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B8" s="4"/>
+      <c r="D8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" s="5"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B9" s="4"/>
+      <c r="D9" t="s">
+        <v>48</v>
+      </c>
+      <c r="F9" s="5"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B10" s="4"/>
+      <c r="D10" t="s">
+        <v>49</v>
+      </c>
+      <c r="F10" s="5"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B11" s="4"/>
+      <c r="D11" t="s">
+        <v>120</v>
+      </c>
+      <c r="F11" s="5"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B12" s="4"/>
+      <c r="D12" t="s">
+        <v>128</v>
+      </c>
+      <c r="F12" s="5"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B13" s="4"/>
+      <c r="D13" t="s">
+        <v>155</v>
+      </c>
+      <c r="F13" s="5"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B14" s="4"/>
+      <c r="D14" t="s">
+        <v>191</v>
+      </c>
+      <c r="F14" s="5"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B15" s="4"/>
+      <c r="D15" t="s">
+        <v>236</v>
+      </c>
+      <c r="F15" s="5"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B16" s="4"/>
+      <c r="D16" s="19" t="s">
+        <v>260</v>
+      </c>
+      <c r="F16" s="5"/>
+      <c r="H16" s="17"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B17" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F17" s="5"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B18" s="4"/>
+      <c r="C18" t="s">
+        <v>35</v>
+      </c>
+      <c r="F18" s="5"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B19" s="4"/>
+      <c r="C19" t="s">
+        <v>97</v>
+      </c>
+      <c r="F19" s="5"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B20" s="4"/>
+      <c r="C20" t="s">
+        <v>168</v>
+      </c>
+      <c r="F20" s="5"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B21" s="4"/>
+      <c r="C21" t="s">
+        <v>182</v>
+      </c>
+      <c r="F21" s="5"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B22" s="4"/>
+      <c r="C22" s="9" t="s">
+        <v>267</v>
+      </c>
+      <c r="F22" s="5"/>
+      <c r="G22" t="s">
+        <v>13</v>
+      </c>
+      <c r="H22" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B23" s="6"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="8"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" s="10" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B27" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="3"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B28" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="C28" s="20"/>
+      <c r="D28" s="20"/>
+      <c r="E28" s="5"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B29" s="4"/>
+      <c r="C29" s="20"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="5"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B30" s="4" t="s">
+        <v>271</v>
+      </c>
+      <c r="C30" s="20"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="5"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B31" s="4"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="20"/>
+      <c r="E31" s="5"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B32" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="C32" s="20"/>
+      <c r="D32" s="20"/>
+      <c r="E32" s="5"/>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B33" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="C33" s="20"/>
+      <c r="D33" s="20"/>
+      <c r="E33" s="5"/>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B34" s="4"/>
+      <c r="C34" s="20"/>
+      <c r="D34" s="20"/>
+      <c r="E34" s="5"/>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B35" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="C35" s="20"/>
+      <c r="D35" s="20"/>
+      <c r="E35" s="5"/>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B36" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="C36" s="20"/>
+      <c r="D36" s="20"/>
+      <c r="E36" s="5"/>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B37" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="C37" s="20"/>
+      <c r="D37" s="20"/>
+      <c r="E37" s="5"/>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B38" s="4"/>
+      <c r="C38" s="20"/>
+      <c r="D38" s="20"/>
+      <c r="E38" s="5"/>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B39" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="C39" s="20"/>
+      <c r="D39" s="20"/>
+      <c r="E39" s="5"/>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B40" s="6"/>
+      <c r="C40" s="7"/>
+      <c r="D40" s="7"/>
+      <c r="E40" s="8"/>
+    </row>
+    <row r="43" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A43" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B43" s="2"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2"/>
+      <c r="G43" s="2"/>
+      <c r="H43" s="2"/>
+      <c r="I43" s="2"/>
+      <c r="J43" s="2"/>
+      <c r="K43" s="2"/>
+      <c r="L43" s="2"/>
+      <c r="M43" s="2"/>
+      <c r="N43" s="2"/>
+      <c r="O43" s="2"/>
+      <c r="P43" s="2"/>
+      <c r="Q43" s="2"/>
+      <c r="R43" s="2"/>
+      <c r="S43" s="3"/>
+    </row>
+    <row r="44" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A44" s="4"/>
+      <c r="B44" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="C44" s="2"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
+      <c r="F44" s="2"/>
+      <c r="G44" s="2"/>
+      <c r="H44" s="2"/>
+      <c r="I44" s="2"/>
+      <c r="J44" s="2"/>
+      <c r="K44" s="2"/>
+      <c r="L44" s="2"/>
+      <c r="M44" s="2"/>
+      <c r="N44" s="2"/>
+      <c r="O44" s="2"/>
+      <c r="P44" s="2"/>
+      <c r="Q44" s="2"/>
+      <c r="R44" s="3"/>
+      <c r="S44" s="5"/>
+    </row>
+    <row r="45" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A45" s="4"/>
+      <c r="B45" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="C45" s="20"/>
+      <c r="D45" s="20"/>
+      <c r="E45" s="20"/>
+      <c r="F45" s="20"/>
+      <c r="G45" s="20"/>
+      <c r="H45" s="20"/>
+      <c r="I45" s="20"/>
+      <c r="J45" s="20"/>
+      <c r="K45" s="20"/>
+      <c r="L45" s="20"/>
+      <c r="M45" s="20"/>
+      <c r="N45" s="20"/>
+      <c r="O45" s="20"/>
+      <c r="P45" s="20"/>
+      <c r="Q45" s="20"/>
+      <c r="R45" s="5"/>
+      <c r="S45" s="5"/>
+    </row>
+    <row r="46" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A46" s="4"/>
+      <c r="B46" s="4"/>
+      <c r="C46" s="20"/>
+      <c r="D46" s="20"/>
+      <c r="E46" s="20"/>
+      <c r="F46" s="20"/>
+      <c r="G46" s="20"/>
+      <c r="H46" s="20"/>
+      <c r="I46" s="20"/>
+      <c r="J46" s="20"/>
+      <c r="K46" s="20"/>
+      <c r="L46" s="20"/>
+      <c r="M46" s="20"/>
+      <c r="N46" s="20"/>
+      <c r="O46" s="20"/>
+      <c r="P46" s="20"/>
+      <c r="Q46" s="20"/>
+      <c r="R46" s="5"/>
+      <c r="S46" s="5"/>
+    </row>
+    <row r="47" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A47" s="4"/>
+      <c r="B47" s="4"/>
+      <c r="C47" s="20"/>
+      <c r="D47" s="20"/>
+      <c r="E47" s="20"/>
+      <c r="F47" s="20"/>
+      <c r="G47" s="20"/>
+      <c r="H47" s="20"/>
+      <c r="I47" s="20"/>
+      <c r="J47" s="20"/>
+      <c r="K47" s="20"/>
+      <c r="L47" s="20"/>
+      <c r="M47" s="20"/>
+      <c r="N47" s="20"/>
+      <c r="O47" s="20"/>
+      <c r="P47" s="20"/>
+      <c r="Q47" s="20"/>
+      <c r="R47" s="5"/>
+      <c r="S47" s="5"/>
+    </row>
+    <row r="48" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A48" s="4"/>
+      <c r="B48" s="4"/>
+      <c r="C48" s="20"/>
+      <c r="D48" s="20"/>
+      <c r="E48" s="20"/>
+      <c r="F48" s="20"/>
+      <c r="G48" s="20"/>
+      <c r="H48" s="20"/>
+      <c r="I48" s="20"/>
+      <c r="J48" s="20"/>
+      <c r="K48" s="20"/>
+      <c r="L48" s="20"/>
+      <c r="M48" s="20"/>
+      <c r="N48" s="20"/>
+      <c r="O48" s="20"/>
+      <c r="P48" s="20"/>
+      <c r="Q48" s="20"/>
+      <c r="R48" s="5"/>
+      <c r="S48" s="5"/>
+    </row>
+    <row r="49" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A49" s="4"/>
+      <c r="B49" s="4"/>
+      <c r="C49" s="20"/>
+      <c r="D49" s="20"/>
+      <c r="E49" s="20"/>
+      <c r="F49" s="20"/>
+      <c r="G49" s="20"/>
+      <c r="H49" s="20"/>
+      <c r="I49" s="20"/>
+      <c r="J49" s="20"/>
+      <c r="K49" s="20"/>
+      <c r="L49" s="20"/>
+      <c r="M49" s="20"/>
+      <c r="N49" s="20"/>
+      <c r="O49" s="20"/>
+      <c r="P49" s="20"/>
+      <c r="Q49" s="20"/>
+      <c r="R49" s="5"/>
+      <c r="S49" s="5"/>
+    </row>
+    <row r="50" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A50" s="4"/>
+      <c r="B50" s="4"/>
+      <c r="C50" s="20"/>
+      <c r="D50" s="20"/>
+      <c r="E50" s="20"/>
+      <c r="F50" s="20"/>
+      <c r="G50" s="20"/>
+      <c r="H50" s="20"/>
+      <c r="I50" s="20"/>
+      <c r="J50" s="20"/>
+      <c r="K50" s="20"/>
+      <c r="L50" s="20"/>
+      <c r="M50" s="20"/>
+      <c r="N50" s="20"/>
+      <c r="O50" s="20"/>
+      <c r="P50" s="20"/>
+      <c r="Q50" s="20"/>
+      <c r="R50" s="5"/>
+      <c r="S50" s="5"/>
+    </row>
+    <row r="51" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A51" s="4"/>
+      <c r="B51" s="4"/>
+      <c r="C51" s="20"/>
+      <c r="D51" s="20"/>
+      <c r="E51" s="20"/>
+      <c r="F51" s="20"/>
+      <c r="G51" s="20"/>
+      <c r="H51" s="20"/>
+      <c r="I51" s="20"/>
+      <c r="J51" s="20"/>
+      <c r="K51" s="20"/>
+      <c r="L51" s="20"/>
+      <c r="M51" s="20"/>
+      <c r="N51" s="20"/>
+      <c r="O51" s="20"/>
+      <c r="P51" s="20"/>
+      <c r="Q51" s="20"/>
+      <c r="R51" s="5"/>
+      <c r="S51" s="5"/>
+    </row>
+    <row r="52" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A52" s="4"/>
+      <c r="B52" s="4"/>
+      <c r="C52" s="20"/>
+      <c r="D52" s="20"/>
+      <c r="E52" s="20"/>
+      <c r="F52" s="20"/>
+      <c r="G52" s="20"/>
+      <c r="H52" s="20"/>
+      <c r="I52" s="20"/>
+      <c r="J52" s="20"/>
+      <c r="K52" s="20"/>
+      <c r="L52" s="20"/>
+      <c r="M52" s="20"/>
+      <c r="N52" s="20"/>
+      <c r="O52" s="20"/>
+      <c r="P52" s="20"/>
+      <c r="Q52" s="20"/>
+      <c r="R52" s="5"/>
+      <c r="S52" s="5"/>
+    </row>
+    <row r="53" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A53" s="4"/>
+      <c r="B53" s="4"/>
+      <c r="C53" s="20"/>
+      <c r="D53" s="20"/>
+      <c r="E53" s="20"/>
+      <c r="F53" s="20"/>
+      <c r="G53" s="20"/>
+      <c r="H53" s="20"/>
+      <c r="I53" s="20"/>
+      <c r="J53" s="20"/>
+      <c r="K53" s="20"/>
+      <c r="L53" s="20"/>
+      <c r="M53" s="20"/>
+      <c r="N53" s="20"/>
+      <c r="O53" s="20"/>
+      <c r="P53" s="20"/>
+      <c r="Q53" s="20"/>
+      <c r="R53" s="5"/>
+      <c r="S53" s="5"/>
+    </row>
+    <row r="54" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A54" s="4"/>
+      <c r="B54" s="6"/>
+      <c r="C54" s="7"/>
+      <c r="D54" s="7"/>
+      <c r="E54" s="7"/>
+      <c r="F54" s="7"/>
+      <c r="G54" s="7"/>
+      <c r="H54" s="7"/>
+      <c r="I54" s="7"/>
+      <c r="J54" s="7"/>
+      <c r="K54" s="7"/>
+      <c r="L54" s="7"/>
+      <c r="M54" s="7"/>
+      <c r="N54" s="7"/>
+      <c r="O54" s="7"/>
+      <c r="P54" s="7"/>
+      <c r="Q54" s="7"/>
+      <c r="R54" s="8"/>
+      <c r="S54" s="5"/>
+    </row>
+    <row r="55" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A55" s="4"/>
+      <c r="B55" s="20"/>
+      <c r="C55" s="20"/>
+      <c r="D55" s="20"/>
+      <c r="E55" s="20"/>
+      <c r="F55" s="20"/>
+      <c r="G55" s="20"/>
+      <c r="H55" s="20"/>
+      <c r="I55" s="20"/>
+      <c r="J55" s="20"/>
+      <c r="K55" s="20"/>
+      <c r="L55" s="20"/>
+      <c r="M55" s="20"/>
+      <c r="N55" s="20"/>
+      <c r="O55" s="20"/>
+      <c r="P55" s="20"/>
+      <c r="Q55" s="20"/>
+      <c r="R55" s="20"/>
+      <c r="S55" s="5"/>
+    </row>
+    <row r="56" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A56" s="4"/>
+      <c r="B56" s="20"/>
+      <c r="C56" s="20"/>
+      <c r="D56" s="20"/>
+      <c r="E56" s="20"/>
+      <c r="F56" s="20"/>
+      <c r="G56" s="20"/>
+      <c r="H56" s="20"/>
+      <c r="I56" s="20"/>
+      <c r="J56" s="20"/>
+      <c r="K56" s="20"/>
+      <c r="L56" s="20"/>
+      <c r="M56" s="20"/>
+      <c r="N56" s="20"/>
+      <c r="O56" s="20"/>
+      <c r="P56" s="20"/>
+      <c r="Q56" s="20"/>
+      <c r="R56" s="20"/>
+      <c r="S56" s="5"/>
+    </row>
+    <row r="57" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A57" s="4"/>
+      <c r="B57" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="C57" s="2"/>
+      <c r="D57" s="2"/>
+      <c r="E57" s="2"/>
+      <c r="F57" s="2"/>
+      <c r="G57" s="2"/>
+      <c r="H57" s="2"/>
+      <c r="I57" s="2"/>
+      <c r="J57" s="2"/>
+      <c r="K57" s="2"/>
+      <c r="L57" s="2"/>
+      <c r="M57" s="2"/>
+      <c r="N57" s="2"/>
+      <c r="O57" s="2"/>
+      <c r="P57" s="2"/>
+      <c r="Q57" s="2"/>
+      <c r="R57" s="3"/>
+      <c r="S57" s="5"/>
+    </row>
+    <row r="58" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A58" s="4"/>
+      <c r="B58" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="C58" s="20"/>
+      <c r="D58" s="20"/>
+      <c r="E58" s="20"/>
+      <c r="F58" s="20"/>
+      <c r="G58" s="20"/>
+      <c r="H58" s="20"/>
+      <c r="I58" s="20"/>
+      <c r="J58" s="20"/>
+      <c r="K58" s="20"/>
+      <c r="L58" s="20"/>
+      <c r="M58" s="20"/>
+      <c r="N58" s="20"/>
+      <c r="O58" s="20"/>
+      <c r="P58" s="20"/>
+      <c r="Q58" s="20"/>
+      <c r="R58" s="5"/>
+      <c r="S58" s="5"/>
+    </row>
+    <row r="59" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A59" s="4"/>
+      <c r="B59" s="4"/>
+      <c r="C59" s="20"/>
+      <c r="D59" s="20"/>
+      <c r="E59" s="20"/>
+      <c r="F59" s="20"/>
+      <c r="G59" s="20"/>
+      <c r="H59" s="20"/>
+      <c r="I59" s="20"/>
+      <c r="J59" s="20"/>
+      <c r="K59" s="20"/>
+      <c r="L59" s="20"/>
+      <c r="M59" s="20"/>
+      <c r="N59" s="20"/>
+      <c r="O59" s="20"/>
+      <c r="P59" s="20"/>
+      <c r="Q59" s="20"/>
+      <c r="R59" s="5"/>
+      <c r="S59" s="5"/>
+    </row>
+    <row r="60" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A60" s="4"/>
+      <c r="B60" s="4"/>
+      <c r="C60" s="20"/>
+      <c r="D60" s="20"/>
+      <c r="E60" s="20"/>
+      <c r="F60" s="20"/>
+      <c r="G60" s="20"/>
+      <c r="H60" s="20"/>
+      <c r="I60" s="20"/>
+      <c r="J60" s="20"/>
+      <c r="K60" s="20"/>
+      <c r="L60" s="20"/>
+      <c r="M60" s="20"/>
+      <c r="N60" s="20"/>
+      <c r="O60" s="20"/>
+      <c r="P60" s="20"/>
+      <c r="Q60" s="20"/>
+      <c r="R60" s="5"/>
+      <c r="S60" s="5"/>
+    </row>
+    <row r="61" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A61" s="4"/>
+      <c r="B61" s="4"/>
+      <c r="C61" s="20"/>
+      <c r="D61" s="20"/>
+      <c r="E61" s="20"/>
+      <c r="F61" s="20"/>
+      <c r="G61" s="20"/>
+      <c r="H61" s="20"/>
+      <c r="I61" s="20"/>
+      <c r="J61" s="20"/>
+      <c r="K61" s="20"/>
+      <c r="L61" s="20"/>
+      <c r="M61" s="20"/>
+      <c r="N61" s="20"/>
+      <c r="O61" s="20"/>
+      <c r="P61" s="20"/>
+      <c r="Q61" s="20"/>
+      <c r="R61" s="5"/>
+      <c r="S61" s="5"/>
+    </row>
+    <row r="62" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A62" s="4"/>
+      <c r="B62" s="4"/>
+      <c r="C62" s="20"/>
+      <c r="D62" s="20"/>
+      <c r="E62" s="20"/>
+      <c r="F62" s="20"/>
+      <c r="G62" s="20"/>
+      <c r="H62" s="20"/>
+      <c r="I62" s="20"/>
+      <c r="J62" s="20"/>
+      <c r="K62" s="20"/>
+      <c r="L62" s="20"/>
+      <c r="M62" s="20"/>
+      <c r="N62" s="20"/>
+      <c r="O62" s="20"/>
+      <c r="P62" s="20"/>
+      <c r="Q62" s="20"/>
+      <c r="R62" s="5"/>
+      <c r="S62" s="5"/>
+    </row>
+    <row r="63" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A63" s="4"/>
+      <c r="B63" s="4"/>
+      <c r="C63" s="20"/>
+      <c r="D63" s="20"/>
+      <c r="E63" s="20"/>
+      <c r="F63" s="20"/>
+      <c r="G63" s="20"/>
+      <c r="H63" s="20"/>
+      <c r="I63" s="20"/>
+      <c r="J63" s="20"/>
+      <c r="K63" s="20"/>
+      <c r="L63" s="20"/>
+      <c r="M63" s="20"/>
+      <c r="N63" s="20"/>
+      <c r="O63" s="20"/>
+      <c r="P63" s="20"/>
+      <c r="Q63" s="20"/>
+      <c r="R63" s="5"/>
+      <c r="S63" s="5"/>
+    </row>
+    <row r="64" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A64" s="4"/>
+      <c r="B64" s="4"/>
+      <c r="C64" s="20"/>
+      <c r="D64" s="20"/>
+      <c r="E64" s="20"/>
+      <c r="F64" s="20"/>
+      <c r="G64" s="20"/>
+      <c r="H64" s="20"/>
+      <c r="I64" s="20"/>
+      <c r="J64" s="20"/>
+      <c r="K64" s="20"/>
+      <c r="L64" s="20"/>
+      <c r="M64" s="20"/>
+      <c r="N64" s="20"/>
+      <c r="O64" s="20"/>
+      <c r="P64" s="20"/>
+      <c r="Q64" s="20"/>
+      <c r="R64" s="5"/>
+      <c r="S64" s="5"/>
+    </row>
+    <row r="65" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A65" s="4"/>
+      <c r="B65" s="4"/>
+      <c r="C65" s="20"/>
+      <c r="D65" s="20"/>
+      <c r="E65" s="20"/>
+      <c r="F65" s="20"/>
+      <c r="G65" s="20"/>
+      <c r="H65" s="20"/>
+      <c r="I65" s="20"/>
+      <c r="J65" s="20"/>
+      <c r="K65" s="20"/>
+      <c r="L65" s="20"/>
+      <c r="M65" s="20"/>
+      <c r="N65" s="20"/>
+      <c r="O65" s="20"/>
+      <c r="P65" s="20"/>
+      <c r="Q65" s="20"/>
+      <c r="R65" s="5"/>
+      <c r="S65" s="5"/>
+    </row>
+    <row r="66" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A66" s="4"/>
+      <c r="B66" s="4"/>
+      <c r="C66" s="20"/>
+      <c r="D66" s="20"/>
+      <c r="E66" s="20"/>
+      <c r="F66" s="20"/>
+      <c r="G66" s="20"/>
+      <c r="H66" s="20"/>
+      <c r="I66" s="20"/>
+      <c r="J66" s="20"/>
+      <c r="K66" s="20"/>
+      <c r="L66" s="20"/>
+      <c r="M66" s="20"/>
+      <c r="N66" s="20"/>
+      <c r="O66" s="20"/>
+      <c r="P66" s="20"/>
+      <c r="Q66" s="20"/>
+      <c r="R66" s="5"/>
+      <c r="S66" s="5"/>
+    </row>
+    <row r="67" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A67" s="4"/>
+      <c r="B67" s="6"/>
+      <c r="C67" s="7"/>
+      <c r="D67" s="7"/>
+      <c r="E67" s="7"/>
+      <c r="F67" s="7"/>
+      <c r="G67" s="7"/>
+      <c r="H67" s="7"/>
+      <c r="I67" s="7"/>
+      <c r="J67" s="7"/>
+      <c r="K67" s="7"/>
+      <c r="L67" s="7"/>
+      <c r="M67" s="7"/>
+      <c r="N67" s="7"/>
+      <c r="O67" s="7"/>
+      <c r="P67" s="7"/>
+      <c r="Q67" s="7"/>
+      <c r="R67" s="8"/>
+      <c r="S67" s="5"/>
+    </row>
+    <row r="68" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A68" s="6"/>
+      <c r="B68" s="7"/>
+      <c r="C68" s="7"/>
+      <c r="D68" s="7"/>
+      <c r="E68" s="7"/>
+      <c r="F68" s="7"/>
+      <c r="G68" s="7"/>
+      <c r="H68" s="7"/>
+      <c r="I68" s="7"/>
+      <c r="J68" s="7"/>
+      <c r="K68" s="7"/>
+      <c r="L68" s="7"/>
+      <c r="M68" s="7"/>
+      <c r="N68" s="7"/>
+      <c r="O68" s="7"/>
+      <c r="P68" s="7"/>
+      <c r="Q68" s="7"/>
+      <c r="R68" s="7"/>
+      <c r="S68" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>